<commit_message>
Ders Listesi import şablon dosyası düzenlendi
</commit_message>
<xml_diff>
--- a/Public/assets/downloads/Ders Listesi.xlsx
+++ b/Public/assets/downloads/Ders Listesi.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Program </t>
   </si>
   <si>
-    <t xml:space="preserve">Dönemi</t>
+    <t xml:space="preserve">Yarıyılı</t>
   </si>
   <si>
     <t xml:space="preserve">Türü</t>
@@ -307,7 +307,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3264,10 +3264,6 @@
       <formula1>"Bilgisayar Teknolojileri,Elektrik ve Enerji,Muhasebe ve Vergi Uygulamaları,Yönetim ve Organizasyon,Finans - Bankacılık ve Sigortacılık,El Sanatları,Seyahat - Turizm ve Eğlence Hizmetleri,Ulaştırma Hizmetleri,Mimarlık Ve Şehir Planlama"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C243" type="whole">
-      <formula1>5</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B243" type="list">
       <formula1>"Bilgisayar Programcılığı,Web Tasarımı ve Kodlama,Elektrik Üretim İletim ve Dağıtım,Alternatif Enerji Kaynakları Teknolojisi,Geleneksel El Sanatları,Kuyumculuk ve Takı Tasarımı,Bankacılık ve Sigortacılık Programı,Maliye,Muhasebe Ve Vergi Uygulamaları,Turiz"</formula1>
       <formula2>0</formula2>
@@ -3278,6 +3274,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J1001" type="list">
       <formula1>"Derslik,Bilgisayar Laboratuvarı,Uzaktan Eğitim Sınıfı,Karma"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="lessThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C1001" type="list">
+      <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Ders listesi şablonu düzenlendi
</commit_message>
<xml_diff>
--- a/Public/assets/downloads/Ders Listesi.xlsx
+++ b/Public/assets/downloads/Ders Listesi.xlsx
@@ -302,12 +302,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J243"/>
+  <dimension ref="A1:J299"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2:C1048576"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3257,15 +3257,179 @@
       <c r="I243" s="4"/>
       <c r="J243" s="3"/>
     </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B244" s="3"/>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B245" s="3"/>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B246" s="3"/>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B247" s="3"/>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B248" s="3"/>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B249" s="3"/>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B250" s="3"/>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B251" s="3"/>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B252" s="3"/>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B253" s="3"/>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B254" s="3"/>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B255" s="3"/>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B256" s="3"/>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B257" s="3"/>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B258" s="3"/>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B259" s="3"/>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B260" s="3"/>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B261" s="3"/>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B262" s="3"/>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B263" s="3"/>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B264" s="3"/>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B265" s="3"/>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B266" s="3"/>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B267" s="3"/>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B268" s="3"/>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B269" s="3"/>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B270" s="3"/>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B271" s="3"/>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B272" s="3"/>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B273" s="3"/>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B274" s="3"/>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B275" s="3"/>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B276" s="3"/>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B277" s="3"/>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B278" s="3"/>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B279" s="3"/>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B280" s="3"/>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B281" s="3"/>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B282" s="3"/>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B283" s="3"/>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B284" s="3"/>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B285" s="3"/>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B286" s="3"/>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B287" s="3"/>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B288" s="3"/>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B289" s="3"/>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B290" s="3"/>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B291" s="3"/>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B292" s="3"/>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B293" s="3"/>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B294" s="3"/>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B295" s="3"/>
+    </row>
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B296" s="3"/>
+    </row>
+    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B297" s="3"/>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B298" s="3"/>
+    </row>
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B299" s="3"/>
+    </row>
   </sheetData>
   <autoFilter ref="B1:J243"/>
   <dataValidations count="5">
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A243" type="list">
       <formula1>"Bilgisayar Teknolojileri,Elektrik ve Enerji,Muhasebe ve Vergi Uygulamaları,Yönetim ve Organizasyon,Finans - Bankacılık ve Sigortacılık,El Sanatları,Seyahat - Turizm ve Eğlence Hizmetleri,Ulaştırma Hizmetleri,Mimarlık Ve Şehir Planlama"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B243" type="list">
-      <formula1>"Bilgisayar Programcılığı,Web Tasarımı ve Kodlama,Elektrik Üretim İletim ve Dağıtım,Alternatif Enerji Kaynakları Teknolojisi,Geleneksel El Sanatları,Kuyumculuk ve Takı Tasarımı,Bankacılık ve Sigortacılık Programı,Maliye,Muhasebe Ve Vergi Uygulamaları,Turiz"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D2:D243" type="list">
@@ -3280,6 +3444,10 @@
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B1:B1001" type="list">
+      <formula1>"Bilgisayar Programcılığı,Web Tasarımı ve Kodlama,Elektrik Üretim İletim ve Dağıtım,Alternatif Enerji Kaynakları Teknolojisi,Geleneksel El Sanatları,Kuyumculuk ve Takı Tasarımı,Bankacılık ve Sigortacılık Programı,Maliye,Muhasebe Ve Vergi Uygulamaları,Turiz"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Ders grup kodu eklemesi yapıldı
</commit_message>
<xml_diff>
--- a/Public/assets/downloads/Ders Listesi.xlsx
+++ b/Public/assets/downloads/Ders Listesi.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -11,7 +11,7 @@
     <sheet name="Sayfa1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sayfa1!$B$1:$J$243</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sayfa1!$B$1:$K$243</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Bölüm </t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dersin Kodu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grup No</t>
   </si>
   <si>
     <t xml:space="preserve">Dersin Adı</t>
@@ -302,23 +305,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J299"/>
+  <dimension ref="A1:K299"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="48.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="48.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,6 +356,9 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
@@ -359,11 +366,12 @@
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="3"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
@@ -371,11 +379,12 @@
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="3"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
@@ -383,11 +392,12 @@
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
@@ -395,11 +405,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
@@ -407,11 +418,12 @@
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
@@ -419,11 +431,12 @@
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
@@ -431,11 +444,12 @@
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
@@ -443,11 +457,12 @@
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
@@ -455,11 +470,12 @@
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
@@ -467,11 +483,12 @@
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
@@ -479,11 +496,12 @@
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
@@ -491,11 +509,12 @@
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
@@ -503,11 +522,12 @@
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
@@ -515,11 +535,12 @@
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="3"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
@@ -527,11 +548,12 @@
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
@@ -539,11 +561,12 @@
       <c r="C17" s="1"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
@@ -551,11 +574,12 @@
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="3"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
@@ -563,11 +587,12 @@
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="3"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
@@ -575,11 +600,12 @@
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="3"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
@@ -587,11 +613,12 @@
       <c r="C21" s="1"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
@@ -599,11 +626,12 @@
       <c r="C22" s="1"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
+      <c r="F22" s="3"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
@@ -611,11 +639,12 @@
       <c r="C23" s="1"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="3"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="3"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
@@ -623,11 +652,12 @@
       <c r="C24" s="1"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
+      <c r="F24" s="3"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
@@ -635,11 +665,12 @@
       <c r="C25" s="1"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
+      <c r="F25" s="3"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="3"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
@@ -647,11 +678,12 @@
       <c r="C26" s="1"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="3"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
@@ -659,11 +691,12 @@
       <c r="C27" s="1"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="3"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="3"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
@@ -671,11 +704,12 @@
       <c r="C28" s="1"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="3"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="3"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
@@ -683,11 +717,12 @@
       <c r="C29" s="1"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="3"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
@@ -695,11 +730,12 @@
       <c r="C30" s="1"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
@@ -707,11 +743,12 @@
       <c r="C31" s="1"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="3"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
@@ -719,11 +756,12 @@
       <c r="C32" s="1"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
+      <c r="F32" s="3"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="3"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
@@ -731,11 +769,12 @@
       <c r="C33" s="1"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
+      <c r="F33" s="3"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="3"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
@@ -743,11 +782,12 @@
       <c r="C34" s="1"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
+      <c r="F34" s="3"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="3"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
@@ -755,11 +795,12 @@
       <c r="C35" s="1"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
+      <c r="F35" s="3"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="3"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
@@ -767,11 +808,12 @@
       <c r="C36" s="1"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
+      <c r="F36" s="3"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="3"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
@@ -783,7 +825,8 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="3"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
@@ -795,7 +838,8 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="3"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
@@ -807,7 +851,8 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="3"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
@@ -819,7 +864,8 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="3"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
@@ -831,7 +877,8 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="3"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
@@ -843,7 +890,8 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="3"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
@@ -855,7 +903,8 @@
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="3"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
@@ -867,7 +916,8 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="3"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
@@ -879,7 +929,8 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="3"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
@@ -891,7 +942,8 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="3"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
@@ -903,7 +955,8 @@
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="3"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
@@ -915,7 +968,8 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="3"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
@@ -927,7 +981,8 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="3"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
@@ -939,7 +994,8 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="3"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
@@ -951,7 +1007,8 @@
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
-      <c r="J51" s="3"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3"/>
@@ -963,7 +1020,8 @@
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
-      <c r="J52" s="3"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3"/>
@@ -975,7 +1033,8 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
-      <c r="J53" s="3"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
@@ -987,7 +1046,8 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
-      <c r="J54" s="3"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3"/>
@@ -999,7 +1059,8 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
-      <c r="J55" s="3"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
@@ -1011,7 +1072,8 @@
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
-      <c r="J56" s="3"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3"/>
@@ -1023,7 +1085,8 @@
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
-      <c r="J57" s="3"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
@@ -1035,7 +1098,8 @@
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
-      <c r="J58" s="3"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
@@ -1047,7 +1111,8 @@
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
-      <c r="J59" s="3"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3"/>
@@ -1055,11 +1120,12 @@
       <c r="C60" s="1"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="4"/>
+      <c r="F60" s="3"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
-      <c r="J60" s="3"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3"/>
@@ -1067,11 +1133,12 @@
       <c r="C61" s="1"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
+      <c r="F61" s="3"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
-      <c r="J61" s="3"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3"/>
@@ -1079,11 +1146,12 @@
       <c r="C62" s="1"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="4"/>
+      <c r="F62" s="3"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
-      <c r="J62" s="3"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3"/>
@@ -1091,11 +1159,12 @@
       <c r="C63" s="1"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
+      <c r="F63" s="3"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
-      <c r="J63" s="3"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3"/>
@@ -1103,11 +1172,12 @@
       <c r="C64" s="1"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
+      <c r="F64" s="3"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
-      <c r="J64" s="3"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3"/>
@@ -1115,11 +1185,12 @@
       <c r="C65" s="1"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
+      <c r="F65" s="3"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="3"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
@@ -1127,11 +1198,12 @@
       <c r="C66" s="1"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="4"/>
+      <c r="F66" s="3"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
-      <c r="J66" s="3"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
@@ -1139,11 +1211,12 @@
       <c r="C67" s="1"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
+      <c r="F67" s="3"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
-      <c r="J67" s="3"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3"/>
@@ -1151,11 +1224,12 @@
       <c r="C68" s="1"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="4"/>
+      <c r="F68" s="3"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
-      <c r="J68" s="3"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3"/>
@@ -1163,11 +1237,12 @@
       <c r="C69" s="1"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
+      <c r="F69" s="3"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
-      <c r="J69" s="3"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3"/>
@@ -1175,11 +1250,12 @@
       <c r="C70" s="1"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
+      <c r="F70" s="3"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
-      <c r="J70" s="3"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3"/>
@@ -1187,11 +1263,12 @@
       <c r="C71" s="1"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
+      <c r="F71" s="3"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
-      <c r="J71" s="3"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3"/>
@@ -1199,11 +1276,12 @@
       <c r="C72" s="1"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="4"/>
+      <c r="F72" s="3"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
-      <c r="J72" s="3"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3"/>
@@ -1211,11 +1289,12 @@
       <c r="C73" s="1"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
+      <c r="F73" s="3"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
-      <c r="J73" s="3"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3"/>
@@ -1223,11 +1302,12 @@
       <c r="C74" s="1"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="4"/>
+      <c r="F74" s="3"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
-      <c r="J74" s="3"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3"/>
@@ -1235,11 +1315,12 @@
       <c r="C75" s="1"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
+      <c r="F75" s="3"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
-      <c r="J75" s="3"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3"/>
@@ -1247,11 +1328,12 @@
       <c r="C76" s="1"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="4"/>
+      <c r="F76" s="3"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
-      <c r="J76" s="3"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3"/>
@@ -1259,11 +1341,12 @@
       <c r="C77" s="1"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
+      <c r="F77" s="3"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
-      <c r="J77" s="3"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3"/>
@@ -1271,11 +1354,12 @@
       <c r="C78" s="1"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="4"/>
+      <c r="F78" s="3"/>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
-      <c r="J78" s="3"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3"/>
@@ -1283,11 +1367,12 @@
       <c r="C79" s="1"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="4"/>
+      <c r="F79" s="3"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
-      <c r="J79" s="3"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3"/>
@@ -1295,11 +1380,12 @@
       <c r="C80" s="1"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
+      <c r="F80" s="3"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
-      <c r="J80" s="3"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3"/>
@@ -1307,11 +1393,12 @@
       <c r="C81" s="1"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="4"/>
+      <c r="F81" s="3"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
-      <c r="J81" s="3"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
@@ -1319,11 +1406,12 @@
       <c r="C82" s="1"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="4"/>
+      <c r="F82" s="3"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
-      <c r="J82" s="3"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3"/>
@@ -1331,11 +1419,12 @@
       <c r="C83" s="1"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="4"/>
+      <c r="F83" s="3"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
-      <c r="J83" s="3"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3"/>
@@ -1343,11 +1432,12 @@
       <c r="C84" s="1"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="4"/>
+      <c r="F84" s="3"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
-      <c r="J84" s="3"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="3"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3"/>
@@ -1355,11 +1445,12 @@
       <c r="C85" s="1"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="4"/>
+      <c r="F85" s="3"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
-      <c r="J85" s="3"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3"/>
@@ -1367,11 +1458,12 @@
       <c r="C86" s="1"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
-      <c r="F86" s="4"/>
+      <c r="F86" s="3"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
-      <c r="J86" s="3"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3"/>
@@ -1379,11 +1471,12 @@
       <c r="C87" s="1"/>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="4"/>
+      <c r="F87" s="3"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
-      <c r="J87" s="3"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3"/>
@@ -1391,11 +1484,12 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="4"/>
+      <c r="F88" s="3"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
-      <c r="J88" s="3"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3"/>
@@ -1403,11 +1497,12 @@
       <c r="C89" s="1"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
-      <c r="F89" s="4"/>
+      <c r="F89" s="3"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
-      <c r="J89" s="3"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3"/>
@@ -1415,11 +1510,12 @@
       <c r="C90" s="1"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="4"/>
+      <c r="F90" s="3"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
-      <c r="J90" s="3"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3"/>
@@ -1427,11 +1523,12 @@
       <c r="C91" s="1"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
+      <c r="F91" s="3"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
-      <c r="J91" s="3"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3"/>
@@ -1439,11 +1536,12 @@
       <c r="C92" s="1"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="4"/>
+      <c r="F92" s="3"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
-      <c r="J92" s="3"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3"/>
@@ -1451,11 +1549,12 @@
       <c r="C93" s="1"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
-      <c r="F93" s="4"/>
+      <c r="F93" s="3"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
-      <c r="J93" s="3"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3"/>
@@ -1463,11 +1562,12 @@
       <c r="C94" s="1"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
-      <c r="F94" s="4"/>
+      <c r="F94" s="3"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
-      <c r="J94" s="3"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3"/>
@@ -1475,11 +1575,12 @@
       <c r="C95" s="1"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="4"/>
+      <c r="F95" s="3"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
-      <c r="J95" s="3"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="3"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3"/>
@@ -1487,11 +1588,12 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
+      <c r="F96" s="3"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
-      <c r="J96" s="3"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="3"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3"/>
@@ -1499,11 +1601,12 @@
       <c r="C97" s="1"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
-      <c r="F97" s="4"/>
+      <c r="F97" s="3"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
-      <c r="J97" s="3"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3"/>
@@ -1511,11 +1614,12 @@
       <c r="C98" s="1"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="4"/>
+      <c r="F98" s="3"/>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
-      <c r="J98" s="3"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="3"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3"/>
@@ -1523,11 +1627,12 @@
       <c r="C99" s="1"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
-      <c r="F99" s="4"/>
+      <c r="F99" s="3"/>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
-      <c r="J99" s="3"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="3"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3"/>
@@ -1535,11 +1640,12 @@
       <c r="C100" s="1"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="4"/>
+      <c r="F100" s="3"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
-      <c r="J100" s="3"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="3"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3"/>
@@ -1547,11 +1653,12 @@
       <c r="C101" s="1"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
-      <c r="F101" s="4"/>
+      <c r="F101" s="3"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
-      <c r="J101" s="3"/>
+      <c r="J101" s="4"/>
+      <c r="K101" s="3"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3"/>
@@ -1559,11 +1666,12 @@
       <c r="C102" s="1"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
-      <c r="F102" s="4"/>
+      <c r="F102" s="3"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
-      <c r="J102" s="3"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="3"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3"/>
@@ -1571,11 +1679,12 @@
       <c r="C103" s="1"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
-      <c r="F103" s="4"/>
+      <c r="F103" s="3"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
-      <c r="J103" s="3"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="3"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3"/>
@@ -1583,11 +1692,12 @@
       <c r="C104" s="1"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
-      <c r="F104" s="4"/>
+      <c r="F104" s="3"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
-      <c r="J104" s="3"/>
+      <c r="J104" s="4"/>
+      <c r="K104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3"/>
@@ -1595,11 +1705,12 @@
       <c r="C105" s="1"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
-      <c r="F105" s="4"/>
+      <c r="F105" s="3"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
-      <c r="J105" s="3"/>
+      <c r="J105" s="4"/>
+      <c r="K105" s="3"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3"/>
@@ -1607,11 +1718,12 @@
       <c r="C106" s="1"/>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
-      <c r="F106" s="4"/>
+      <c r="F106" s="3"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
-      <c r="J106" s="3"/>
+      <c r="J106" s="4"/>
+      <c r="K106" s="3"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3"/>
@@ -1619,11 +1731,12 @@
       <c r="C107" s="1"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
-      <c r="F107" s="4"/>
+      <c r="F107" s="3"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
-      <c r="J107" s="3"/>
+      <c r="J107" s="4"/>
+      <c r="K107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3"/>
@@ -1631,11 +1744,12 @@
       <c r="C108" s="1"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
-      <c r="F108" s="4"/>
+      <c r="F108" s="3"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
-      <c r="J108" s="3"/>
+      <c r="J108" s="4"/>
+      <c r="K108" s="3"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3"/>
@@ -1643,11 +1757,12 @@
       <c r="C109" s="1"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
-      <c r="F109" s="4"/>
+      <c r="F109" s="3"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
-      <c r="J109" s="3"/>
+      <c r="J109" s="4"/>
+      <c r="K109" s="3"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3"/>
@@ -1655,11 +1770,12 @@
       <c r="C110" s="1"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
-      <c r="F110" s="4"/>
+      <c r="F110" s="3"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
-      <c r="J110" s="3"/>
+      <c r="J110" s="4"/>
+      <c r="K110" s="3"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3"/>
@@ -1667,11 +1783,12 @@
       <c r="C111" s="1"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
-      <c r="F111" s="4"/>
+      <c r="F111" s="3"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
-      <c r="J111" s="3"/>
+      <c r="J111" s="4"/>
+      <c r="K111" s="3"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3"/>
@@ -1679,11 +1796,12 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
-      <c r="F112" s="4"/>
+      <c r="F112" s="3"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
-      <c r="J112" s="3"/>
+      <c r="J112" s="4"/>
+      <c r="K112" s="3"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3"/>
@@ -1691,11 +1809,12 @@
       <c r="C113" s="1"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
-      <c r="F113" s="4"/>
+      <c r="F113" s="3"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
       <c r="I113" s="4"/>
-      <c r="J113" s="3"/>
+      <c r="J113" s="4"/>
+      <c r="K113" s="3"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3"/>
@@ -1703,11 +1822,12 @@
       <c r="C114" s="1"/>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
-      <c r="F114" s="4"/>
+      <c r="F114" s="3"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
-      <c r="J114" s="3"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="3"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3"/>
@@ -1715,11 +1835,12 @@
       <c r="C115" s="1"/>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
-      <c r="F115" s="4"/>
+      <c r="F115" s="3"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
-      <c r="J115" s="3"/>
+      <c r="J115" s="4"/>
+      <c r="K115" s="3"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3"/>
@@ -1727,11 +1848,12 @@
       <c r="C116" s="1"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
-      <c r="F116" s="4"/>
+      <c r="F116" s="3"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
-      <c r="J116" s="3"/>
+      <c r="J116" s="4"/>
+      <c r="K116" s="3"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3"/>
@@ -1739,11 +1861,12 @@
       <c r="C117" s="1"/>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
-      <c r="F117" s="4"/>
+      <c r="F117" s="3"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
-      <c r="J117" s="3"/>
+      <c r="J117" s="4"/>
+      <c r="K117" s="3"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3"/>
@@ -1751,11 +1874,12 @@
       <c r="C118" s="1"/>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
-      <c r="F118" s="4"/>
+      <c r="F118" s="3"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
-      <c r="J118" s="3"/>
+      <c r="J118" s="4"/>
+      <c r="K118" s="3"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3"/>
@@ -1763,11 +1887,12 @@
       <c r="C119" s="1"/>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
-      <c r="F119" s="4"/>
+      <c r="F119" s="3"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
-      <c r="J119" s="3"/>
+      <c r="J119" s="4"/>
+      <c r="K119" s="3"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3"/>
@@ -1775,11 +1900,12 @@
       <c r="C120" s="1"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
-      <c r="F120" s="4"/>
+      <c r="F120" s="3"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
-      <c r="J120" s="3"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="3"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3"/>
@@ -1787,11 +1913,12 @@
       <c r="C121" s="1"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
-      <c r="F121" s="4"/>
+      <c r="F121" s="3"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
-      <c r="J121" s="3"/>
+      <c r="J121" s="4"/>
+      <c r="K121" s="3"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3"/>
@@ -1799,11 +1926,12 @@
       <c r="C122" s="1"/>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
-      <c r="F122" s="4"/>
+      <c r="F122" s="3"/>
       <c r="G122" s="4"/>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
-      <c r="J122" s="3"/>
+      <c r="J122" s="4"/>
+      <c r="K122" s="3"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3"/>
@@ -1811,11 +1939,12 @@
       <c r="C123" s="1"/>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
-      <c r="F123" s="4"/>
+      <c r="F123" s="3"/>
       <c r="G123" s="4"/>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
-      <c r="J123" s="3"/>
+      <c r="J123" s="4"/>
+      <c r="K123" s="3"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3"/>
@@ -1823,11 +1952,12 @@
       <c r="C124" s="1"/>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
-      <c r="F124" s="4"/>
+      <c r="F124" s="3"/>
       <c r="G124" s="4"/>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
-      <c r="J124" s="3"/>
+      <c r="J124" s="4"/>
+      <c r="K124" s="3"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3"/>
@@ -1835,11 +1965,12 @@
       <c r="C125" s="1"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
-      <c r="F125" s="4"/>
+      <c r="F125" s="3"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
-      <c r="J125" s="3"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="3"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3"/>
@@ -1847,11 +1978,12 @@
       <c r="C126" s="1"/>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
-      <c r="F126" s="4"/>
+      <c r="F126" s="3"/>
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
-      <c r="J126" s="3"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3"/>
@@ -1859,11 +1991,12 @@
       <c r="C127" s="1"/>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
-      <c r="F127" s="4"/>
+      <c r="F127" s="3"/>
       <c r="G127" s="4"/>
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
-      <c r="J127" s="3"/>
+      <c r="J127" s="4"/>
+      <c r="K127" s="3"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3"/>
@@ -1871,11 +2004,12 @@
       <c r="C128" s="1"/>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
-      <c r="F128" s="4"/>
+      <c r="F128" s="3"/>
       <c r="G128" s="4"/>
       <c r="H128" s="4"/>
       <c r="I128" s="4"/>
-      <c r="J128" s="3"/>
+      <c r="J128" s="4"/>
+      <c r="K128" s="3"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3"/>
@@ -1883,11 +2017,12 @@
       <c r="C129" s="1"/>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
-      <c r="F129" s="4"/>
+      <c r="F129" s="3"/>
       <c r="G129" s="4"/>
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
-      <c r="J129" s="3"/>
+      <c r="J129" s="4"/>
+      <c r="K129" s="3"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3"/>
@@ -1895,11 +2030,12 @@
       <c r="C130" s="1"/>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
-      <c r="F130" s="4"/>
+      <c r="F130" s="3"/>
       <c r="G130" s="4"/>
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
-      <c r="J130" s="3"/>
+      <c r="J130" s="4"/>
+      <c r="K130" s="3"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="3"/>
@@ -1907,11 +2043,12 @@
       <c r="C131" s="1"/>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
-      <c r="F131" s="4"/>
+      <c r="F131" s="3"/>
       <c r="G131" s="4"/>
       <c r="H131" s="4"/>
       <c r="I131" s="4"/>
-      <c r="J131" s="3"/>
+      <c r="J131" s="4"/>
+      <c r="K131" s="3"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3"/>
@@ -1919,11 +2056,12 @@
       <c r="C132" s="1"/>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
-      <c r="F132" s="4"/>
+      <c r="F132" s="3"/>
       <c r="G132" s="4"/>
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
-      <c r="J132" s="3"/>
+      <c r="J132" s="4"/>
+      <c r="K132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3"/>
@@ -1931,11 +2069,12 @@
       <c r="C133" s="1"/>
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
-      <c r="F133" s="4"/>
+      <c r="F133" s="3"/>
       <c r="G133" s="4"/>
       <c r="H133" s="4"/>
       <c r="I133" s="4"/>
-      <c r="J133" s="3"/>
+      <c r="J133" s="4"/>
+      <c r="K133" s="3"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3"/>
@@ -1943,11 +2082,12 @@
       <c r="C134" s="1"/>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
-      <c r="F134" s="4"/>
+      <c r="F134" s="3"/>
       <c r="G134" s="4"/>
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
-      <c r="J134" s="3"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="3"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3"/>
@@ -1955,11 +2095,12 @@
       <c r="C135" s="1"/>
       <c r="D135" s="3"/>
       <c r="E135" s="3"/>
-      <c r="F135" s="4"/>
+      <c r="F135" s="3"/>
       <c r="G135" s="4"/>
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
-      <c r="J135" s="3"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="3"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3"/>
@@ -1967,11 +2108,12 @@
       <c r="C136" s="1"/>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
-      <c r="F136" s="4"/>
+      <c r="F136" s="3"/>
       <c r="G136" s="4"/>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
-      <c r="J136" s="3"/>
+      <c r="J136" s="4"/>
+      <c r="K136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3"/>
@@ -1979,11 +2121,12 @@
       <c r="C137" s="1"/>
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>
-      <c r="F137" s="4"/>
+      <c r="F137" s="3"/>
       <c r="G137" s="4"/>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
-      <c r="J137" s="3"/>
+      <c r="J137" s="4"/>
+      <c r="K137" s="3"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3"/>
@@ -1991,11 +2134,12 @@
       <c r="C138" s="1"/>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
-      <c r="F138" s="4"/>
+      <c r="F138" s="3"/>
       <c r="G138" s="4"/>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
-      <c r="J138" s="3"/>
+      <c r="J138" s="4"/>
+      <c r="K138" s="3"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3"/>
@@ -2003,11 +2147,12 @@
       <c r="C139" s="1"/>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
-      <c r="F139" s="4"/>
+      <c r="F139" s="3"/>
       <c r="G139" s="4"/>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
-      <c r="J139" s="3"/>
+      <c r="J139" s="4"/>
+      <c r="K139" s="3"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3"/>
@@ -2015,11 +2160,12 @@
       <c r="C140" s="1"/>
       <c r="D140" s="3"/>
       <c r="E140" s="3"/>
-      <c r="F140" s="4"/>
+      <c r="F140" s="3"/>
       <c r="G140" s="4"/>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
-      <c r="J140" s="3"/>
+      <c r="J140" s="4"/>
+      <c r="K140" s="3"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3"/>
@@ -2027,11 +2173,12 @@
       <c r="C141" s="1"/>
       <c r="D141" s="3"/>
       <c r="E141" s="3"/>
-      <c r="F141" s="4"/>
+      <c r="F141" s="3"/>
       <c r="G141" s="4"/>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
-      <c r="J141" s="3"/>
+      <c r="J141" s="4"/>
+      <c r="K141" s="3"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3"/>
@@ -2039,11 +2186,12 @@
       <c r="C142" s="1"/>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
-      <c r="F142" s="4"/>
+      <c r="F142" s="3"/>
       <c r="G142" s="4"/>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
-      <c r="J142" s="3"/>
+      <c r="J142" s="4"/>
+      <c r="K142" s="3"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3"/>
@@ -2051,11 +2199,12 @@
       <c r="C143" s="1"/>
       <c r="D143" s="3"/>
       <c r="E143" s="3"/>
-      <c r="F143" s="4"/>
+      <c r="F143" s="3"/>
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
-      <c r="J143" s="3"/>
+      <c r="J143" s="4"/>
+      <c r="K143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3"/>
@@ -2063,11 +2212,12 @@
       <c r="C144" s="1"/>
       <c r="D144" s="3"/>
       <c r="E144" s="3"/>
-      <c r="F144" s="4"/>
+      <c r="F144" s="3"/>
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
-      <c r="J144" s="3"/>
+      <c r="J144" s="4"/>
+      <c r="K144" s="3"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3"/>
@@ -2075,11 +2225,12 @@
       <c r="C145" s="1"/>
       <c r="D145" s="3"/>
       <c r="E145" s="3"/>
-      <c r="F145" s="4"/>
+      <c r="F145" s="3"/>
       <c r="G145" s="4"/>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
-      <c r="J145" s="3"/>
+      <c r="J145" s="4"/>
+      <c r="K145" s="3"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3"/>
@@ -2087,11 +2238,12 @@
       <c r="C146" s="1"/>
       <c r="D146" s="3"/>
       <c r="E146" s="3"/>
-      <c r="F146" s="4"/>
+      <c r="F146" s="3"/>
       <c r="G146" s="4"/>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
-      <c r="J146" s="3"/>
+      <c r="J146" s="4"/>
+      <c r="K146" s="3"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3"/>
@@ -2099,11 +2251,12 @@
       <c r="C147" s="1"/>
       <c r="D147" s="3"/>
       <c r="E147" s="3"/>
-      <c r="F147" s="4"/>
+      <c r="F147" s="3"/>
       <c r="G147" s="4"/>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
-      <c r="J147" s="3"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="3"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3"/>
@@ -2111,11 +2264,12 @@
       <c r="C148" s="1"/>
       <c r="D148" s="3"/>
       <c r="E148" s="3"/>
-      <c r="F148" s="4"/>
+      <c r="F148" s="3"/>
       <c r="G148" s="4"/>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
-      <c r="J148" s="3"/>
+      <c r="J148" s="4"/>
+      <c r="K148" s="3"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3"/>
@@ -2123,11 +2277,12 @@
       <c r="C149" s="1"/>
       <c r="D149" s="3"/>
       <c r="E149" s="3"/>
-      <c r="F149" s="4"/>
+      <c r="F149" s="3"/>
       <c r="G149" s="4"/>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
-      <c r="J149" s="3"/>
+      <c r="J149" s="4"/>
+      <c r="K149" s="3"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3"/>
@@ -2135,11 +2290,12 @@
       <c r="C150" s="1"/>
       <c r="D150" s="3"/>
       <c r="E150" s="3"/>
-      <c r="F150" s="4"/>
+      <c r="F150" s="3"/>
       <c r="G150" s="4"/>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
-      <c r="J150" s="3"/>
+      <c r="J150" s="4"/>
+      <c r="K150" s="3"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3"/>
@@ -2147,11 +2303,12 @@
       <c r="C151" s="1"/>
       <c r="D151" s="3"/>
       <c r="E151" s="3"/>
-      <c r="F151" s="4"/>
+      <c r="F151" s="3"/>
       <c r="G151" s="4"/>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
-      <c r="J151" s="3"/>
+      <c r="J151" s="4"/>
+      <c r="K151" s="3"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3"/>
@@ -2159,11 +2316,12 @@
       <c r="C152" s="1"/>
       <c r="D152" s="3"/>
       <c r="E152" s="3"/>
-      <c r="F152" s="4"/>
+      <c r="F152" s="3"/>
       <c r="G152" s="4"/>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
-      <c r="J152" s="3"/>
+      <c r="J152" s="4"/>
+      <c r="K152" s="3"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3"/>
@@ -2171,11 +2329,12 @@
       <c r="C153" s="1"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
-      <c r="F153" s="4"/>
+      <c r="F153" s="3"/>
       <c r="G153" s="4"/>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
-      <c r="J153" s="3"/>
+      <c r="J153" s="4"/>
+      <c r="K153" s="3"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3"/>
@@ -2183,11 +2342,12 @@
       <c r="C154" s="1"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
-      <c r="F154" s="4"/>
+      <c r="F154" s="3"/>
       <c r="G154" s="4"/>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
-      <c r="J154" s="3"/>
+      <c r="J154" s="4"/>
+      <c r="K154" s="3"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3"/>
@@ -2195,11 +2355,12 @@
       <c r="C155" s="1"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
-      <c r="F155" s="4"/>
+      <c r="F155" s="3"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
-      <c r="J155" s="3"/>
+      <c r="J155" s="4"/>
+      <c r="K155" s="3"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="3"/>
@@ -2207,11 +2368,12 @@
       <c r="C156" s="1"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
-      <c r="F156" s="4"/>
+      <c r="F156" s="3"/>
       <c r="G156" s="4"/>
       <c r="H156" s="4"/>
       <c r="I156" s="4"/>
-      <c r="J156" s="3"/>
+      <c r="J156" s="4"/>
+      <c r="K156" s="3"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="3"/>
@@ -2219,11 +2381,12 @@
       <c r="C157" s="1"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
-      <c r="F157" s="4"/>
+      <c r="F157" s="3"/>
       <c r="G157" s="4"/>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
-      <c r="J157" s="3"/>
+      <c r="J157" s="4"/>
+      <c r="K157" s="3"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="3"/>
@@ -2231,11 +2394,12 @@
       <c r="C158" s="1"/>
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
-      <c r="F158" s="4"/>
+      <c r="F158" s="3"/>
       <c r="G158" s="4"/>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
-      <c r="J158" s="3"/>
+      <c r="J158" s="4"/>
+      <c r="K158" s="3"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3"/>
@@ -2243,11 +2407,12 @@
       <c r="C159" s="1"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
-      <c r="F159" s="4"/>
+      <c r="F159" s="3"/>
       <c r="G159" s="4"/>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
-      <c r="J159" s="3"/>
+      <c r="J159" s="4"/>
+      <c r="K159" s="3"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3"/>
@@ -2255,11 +2420,12 @@
       <c r="C160" s="1"/>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
-      <c r="F160" s="4"/>
+      <c r="F160" s="3"/>
       <c r="G160" s="4"/>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
-      <c r="J160" s="3"/>
+      <c r="J160" s="4"/>
+      <c r="K160" s="3"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="3"/>
@@ -2267,11 +2433,12 @@
       <c r="C161" s="1"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
-      <c r="F161" s="4"/>
+      <c r="F161" s="3"/>
       <c r="G161" s="4"/>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
-      <c r="J161" s="3"/>
+      <c r="J161" s="4"/>
+      <c r="K161" s="3"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="3"/>
@@ -2279,11 +2446,12 @@
       <c r="C162" s="1"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
-      <c r="F162" s="4"/>
+      <c r="F162" s="3"/>
       <c r="G162" s="4"/>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
-      <c r="J162" s="3"/>
+      <c r="J162" s="4"/>
+      <c r="K162" s="3"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="3"/>
@@ -2291,11 +2459,12 @@
       <c r="C163" s="1"/>
       <c r="D163" s="3"/>
       <c r="E163" s="3"/>
-      <c r="F163" s="4"/>
+      <c r="F163" s="3"/>
       <c r="G163" s="4"/>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
-      <c r="J163" s="3"/>
+      <c r="J163" s="4"/>
+      <c r="K163" s="3"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="3"/>
@@ -2303,11 +2472,12 @@
       <c r="C164" s="1"/>
       <c r="D164" s="3"/>
       <c r="E164" s="3"/>
-      <c r="F164" s="4"/>
+      <c r="F164" s="3"/>
       <c r="G164" s="4"/>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
-      <c r="J164" s="3"/>
+      <c r="J164" s="4"/>
+      <c r="K164" s="3"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="3"/>
@@ -2315,11 +2485,12 @@
       <c r="C165" s="1"/>
       <c r="D165" s="3"/>
       <c r="E165" s="3"/>
-      <c r="F165" s="4"/>
+      <c r="F165" s="3"/>
       <c r="G165" s="4"/>
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
-      <c r="J165" s="3"/>
+      <c r="J165" s="4"/>
+      <c r="K165" s="3"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="3"/>
@@ -2327,11 +2498,12 @@
       <c r="C166" s="1"/>
       <c r="D166" s="3"/>
       <c r="E166" s="3"/>
-      <c r="F166" s="4"/>
+      <c r="F166" s="3"/>
       <c r="G166" s="4"/>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
-      <c r="J166" s="3"/>
+      <c r="J166" s="4"/>
+      <c r="K166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="3"/>
@@ -2339,11 +2511,12 @@
       <c r="C167" s="1"/>
       <c r="D167" s="3"/>
       <c r="E167" s="3"/>
-      <c r="F167" s="4"/>
+      <c r="F167" s="3"/>
       <c r="G167" s="4"/>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
-      <c r="J167" s="3"/>
+      <c r="J167" s="4"/>
+      <c r="K167" s="3"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="3"/>
@@ -2351,11 +2524,12 @@
       <c r="C168" s="1"/>
       <c r="D168" s="3"/>
       <c r="E168" s="3"/>
-      <c r="F168" s="4"/>
+      <c r="F168" s="3"/>
       <c r="G168" s="4"/>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
-      <c r="J168" s="3"/>
+      <c r="J168" s="4"/>
+      <c r="K168" s="3"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="3"/>
@@ -2363,11 +2537,12 @@
       <c r="C169" s="1"/>
       <c r="D169" s="3"/>
       <c r="E169" s="3"/>
-      <c r="F169" s="4"/>
+      <c r="F169" s="3"/>
       <c r="G169" s="4"/>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
-      <c r="J169" s="3"/>
+      <c r="J169" s="4"/>
+      <c r="K169" s="3"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="3"/>
@@ -2375,11 +2550,12 @@
       <c r="C170" s="1"/>
       <c r="D170" s="3"/>
       <c r="E170" s="3"/>
-      <c r="F170" s="4"/>
+      <c r="F170" s="3"/>
       <c r="G170" s="4"/>
       <c r="H170" s="4"/>
       <c r="I170" s="4"/>
-      <c r="J170" s="3"/>
+      <c r="J170" s="4"/>
+      <c r="K170" s="3"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="3"/>
@@ -2387,11 +2563,12 @@
       <c r="C171" s="1"/>
       <c r="D171" s="3"/>
       <c r="E171" s="3"/>
-      <c r="F171" s="4"/>
+      <c r="F171" s="3"/>
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
-      <c r="J171" s="3"/>
+      <c r="J171" s="4"/>
+      <c r="K171" s="3"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="3"/>
@@ -2399,11 +2576,12 @@
       <c r="C172" s="1"/>
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
-      <c r="F172" s="4"/>
+      <c r="F172" s="3"/>
       <c r="G172" s="4"/>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
-      <c r="J172" s="3"/>
+      <c r="J172" s="4"/>
+      <c r="K172" s="3"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="3"/>
@@ -2411,11 +2589,12 @@
       <c r="C173" s="1"/>
       <c r="D173" s="3"/>
       <c r="E173" s="3"/>
-      <c r="F173" s="4"/>
+      <c r="F173" s="3"/>
       <c r="G173" s="4"/>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
-      <c r="J173" s="3"/>
+      <c r="J173" s="4"/>
+      <c r="K173" s="3"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="3"/>
@@ -2423,11 +2602,12 @@
       <c r="C174" s="1"/>
       <c r="D174" s="3"/>
       <c r="E174" s="3"/>
-      <c r="F174" s="4"/>
+      <c r="F174" s="3"/>
       <c r="G174" s="4"/>
       <c r="H174" s="4"/>
       <c r="I174" s="4"/>
-      <c r="J174" s="3"/>
+      <c r="J174" s="4"/>
+      <c r="K174" s="3"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="3"/>
@@ -2435,11 +2615,12 @@
       <c r="C175" s="1"/>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
-      <c r="F175" s="4"/>
+      <c r="F175" s="3"/>
       <c r="G175" s="4"/>
       <c r="H175" s="4"/>
       <c r="I175" s="4"/>
-      <c r="J175" s="3"/>
+      <c r="J175" s="4"/>
+      <c r="K175" s="3"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="3"/>
@@ -2447,11 +2628,12 @@
       <c r="C176" s="1"/>
       <c r="D176" s="3"/>
       <c r="E176" s="3"/>
-      <c r="F176" s="4"/>
+      <c r="F176" s="3"/>
       <c r="G176" s="4"/>
       <c r="H176" s="4"/>
       <c r="I176" s="4"/>
-      <c r="J176" s="3"/>
+      <c r="J176" s="4"/>
+      <c r="K176" s="3"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="3"/>
@@ -2459,11 +2641,12 @@
       <c r="C177" s="1"/>
       <c r="D177" s="3"/>
       <c r="E177" s="3"/>
-      <c r="F177" s="4"/>
+      <c r="F177" s="3"/>
       <c r="G177" s="4"/>
       <c r="H177" s="4"/>
       <c r="I177" s="4"/>
-      <c r="J177" s="3"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="3"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="3"/>
@@ -2471,11 +2654,12 @@
       <c r="C178" s="1"/>
       <c r="D178" s="3"/>
       <c r="E178" s="3"/>
-      <c r="F178" s="4"/>
+      <c r="F178" s="3"/>
       <c r="G178" s="4"/>
       <c r="H178" s="4"/>
       <c r="I178" s="4"/>
-      <c r="J178" s="3"/>
+      <c r="J178" s="4"/>
+      <c r="K178" s="3"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="3"/>
@@ -2483,11 +2667,12 @@
       <c r="C179" s="1"/>
       <c r="D179" s="3"/>
       <c r="E179" s="3"/>
-      <c r="F179" s="4"/>
+      <c r="F179" s="3"/>
       <c r="G179" s="4"/>
       <c r="H179" s="4"/>
       <c r="I179" s="4"/>
-      <c r="J179" s="3"/>
+      <c r="J179" s="4"/>
+      <c r="K179" s="3"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="3"/>
@@ -2495,11 +2680,12 @@
       <c r="C180" s="1"/>
       <c r="D180" s="3"/>
       <c r="E180" s="3"/>
-      <c r="F180" s="4"/>
+      <c r="F180" s="3"/>
       <c r="G180" s="4"/>
       <c r="H180" s="4"/>
       <c r="I180" s="4"/>
-      <c r="J180" s="3"/>
+      <c r="J180" s="4"/>
+      <c r="K180" s="3"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="3"/>
@@ -2507,11 +2693,12 @@
       <c r="C181" s="1"/>
       <c r="D181" s="3"/>
       <c r="E181" s="3"/>
-      <c r="F181" s="4"/>
+      <c r="F181" s="3"/>
       <c r="G181" s="4"/>
       <c r="H181" s="4"/>
       <c r="I181" s="4"/>
-      <c r="J181" s="3"/>
+      <c r="J181" s="4"/>
+      <c r="K181" s="3"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="3"/>
@@ -2519,11 +2706,12 @@
       <c r="C182" s="1"/>
       <c r="D182" s="3"/>
       <c r="E182" s="3"/>
-      <c r="F182" s="4"/>
+      <c r="F182" s="3"/>
       <c r="G182" s="4"/>
       <c r="H182" s="4"/>
       <c r="I182" s="4"/>
-      <c r="J182" s="3"/>
+      <c r="J182" s="4"/>
+      <c r="K182" s="3"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="3"/>
@@ -2531,11 +2719,12 @@
       <c r="C183" s="1"/>
       <c r="D183" s="3"/>
       <c r="E183" s="3"/>
-      <c r="F183" s="4"/>
+      <c r="F183" s="3"/>
       <c r="G183" s="4"/>
       <c r="H183" s="4"/>
       <c r="I183" s="4"/>
-      <c r="J183" s="3"/>
+      <c r="J183" s="4"/>
+      <c r="K183" s="3"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="3"/>
@@ -2543,11 +2732,12 @@
       <c r="C184" s="1"/>
       <c r="D184" s="3"/>
       <c r="E184" s="3"/>
-      <c r="F184" s="4"/>
+      <c r="F184" s="3"/>
       <c r="G184" s="4"/>
       <c r="H184" s="4"/>
       <c r="I184" s="4"/>
-      <c r="J184" s="3"/>
+      <c r="J184" s="4"/>
+      <c r="K184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="3"/>
@@ -2555,11 +2745,12 @@
       <c r="C185" s="1"/>
       <c r="D185" s="3"/>
       <c r="E185" s="3"/>
-      <c r="F185" s="4"/>
+      <c r="F185" s="3"/>
       <c r="G185" s="4"/>
       <c r="H185" s="4"/>
       <c r="I185" s="4"/>
-      <c r="J185" s="3"/>
+      <c r="J185" s="4"/>
+      <c r="K185" s="3"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="3"/>
@@ -2567,11 +2758,12 @@
       <c r="C186" s="1"/>
       <c r="D186" s="3"/>
       <c r="E186" s="3"/>
-      <c r="F186" s="4"/>
+      <c r="F186" s="3"/>
       <c r="G186" s="4"/>
       <c r="H186" s="4"/>
       <c r="I186" s="4"/>
-      <c r="J186" s="3"/>
+      <c r="J186" s="4"/>
+      <c r="K186" s="3"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="3"/>
@@ -2579,11 +2771,12 @@
       <c r="C187" s="1"/>
       <c r="D187" s="3"/>
       <c r="E187" s="3"/>
-      <c r="F187" s="4"/>
+      <c r="F187" s="3"/>
       <c r="G187" s="4"/>
       <c r="H187" s="4"/>
       <c r="I187" s="4"/>
-      <c r="J187" s="3"/>
+      <c r="J187" s="4"/>
+      <c r="K187" s="3"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="3"/>
@@ -2591,11 +2784,12 @@
       <c r="C188" s="1"/>
       <c r="D188" s="3"/>
       <c r="E188" s="3"/>
-      <c r="F188" s="4"/>
+      <c r="F188" s="3"/>
       <c r="G188" s="4"/>
       <c r="H188" s="4"/>
       <c r="I188" s="4"/>
-      <c r="J188" s="3"/>
+      <c r="J188" s="4"/>
+      <c r="K188" s="3"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="3"/>
@@ -2603,11 +2797,12 @@
       <c r="C189" s="1"/>
       <c r="D189" s="3"/>
       <c r="E189" s="3"/>
-      <c r="F189" s="4"/>
+      <c r="F189" s="3"/>
       <c r="G189" s="4"/>
       <c r="H189" s="4"/>
       <c r="I189" s="4"/>
-      <c r="J189" s="3"/>
+      <c r="J189" s="4"/>
+      <c r="K189" s="3"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="3"/>
@@ -2615,11 +2810,12 @@
       <c r="C190" s="1"/>
       <c r="D190" s="3"/>
       <c r="E190" s="3"/>
-      <c r="F190" s="4"/>
+      <c r="F190" s="3"/>
       <c r="G190" s="4"/>
       <c r="H190" s="4"/>
       <c r="I190" s="4"/>
-      <c r="J190" s="3"/>
+      <c r="J190" s="4"/>
+      <c r="K190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="3"/>
@@ -2627,11 +2823,12 @@
       <c r="C191" s="1"/>
       <c r="D191" s="3"/>
       <c r="E191" s="3"/>
-      <c r="F191" s="4"/>
+      <c r="F191" s="3"/>
       <c r="G191" s="4"/>
       <c r="H191" s="4"/>
       <c r="I191" s="4"/>
-      <c r="J191" s="3"/>
+      <c r="J191" s="4"/>
+      <c r="K191" s="3"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="3"/>
@@ -2639,11 +2836,12 @@
       <c r="C192" s="1"/>
       <c r="D192" s="3"/>
       <c r="E192" s="3"/>
-      <c r="F192" s="4"/>
+      <c r="F192" s="3"/>
       <c r="G192" s="4"/>
       <c r="H192" s="4"/>
       <c r="I192" s="4"/>
-      <c r="J192" s="3"/>
+      <c r="J192" s="4"/>
+      <c r="K192" s="3"/>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="3"/>
@@ -2651,11 +2849,12 @@
       <c r="C193" s="1"/>
       <c r="D193" s="3"/>
       <c r="E193" s="3"/>
-      <c r="F193" s="4"/>
+      <c r="F193" s="3"/>
       <c r="G193" s="4"/>
       <c r="H193" s="4"/>
       <c r="I193" s="4"/>
-      <c r="J193" s="3"/>
+      <c r="J193" s="4"/>
+      <c r="K193" s="3"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="3"/>
@@ -2663,11 +2862,12 @@
       <c r="C194" s="1"/>
       <c r="D194" s="3"/>
       <c r="E194" s="3"/>
-      <c r="F194" s="4"/>
+      <c r="F194" s="3"/>
       <c r="G194" s="4"/>
       <c r="H194" s="4"/>
       <c r="I194" s="4"/>
-      <c r="J194" s="3"/>
+      <c r="J194" s="4"/>
+      <c r="K194" s="3"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="3"/>
@@ -2675,11 +2875,12 @@
       <c r="C195" s="1"/>
       <c r="D195" s="3"/>
       <c r="E195" s="3"/>
-      <c r="F195" s="4"/>
+      <c r="F195" s="3"/>
       <c r="G195" s="4"/>
       <c r="H195" s="4"/>
       <c r="I195" s="4"/>
-      <c r="J195" s="3"/>
+      <c r="J195" s="4"/>
+      <c r="K195" s="3"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="3"/>
@@ -2687,11 +2888,12 @@
       <c r="C196" s="1"/>
       <c r="D196" s="3"/>
       <c r="E196" s="3"/>
-      <c r="F196" s="4"/>
+      <c r="F196" s="3"/>
       <c r="G196" s="4"/>
       <c r="H196" s="4"/>
       <c r="I196" s="4"/>
-      <c r="J196" s="3"/>
+      <c r="J196" s="4"/>
+      <c r="K196" s="3"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="3"/>
@@ -2699,11 +2901,12 @@
       <c r="C197" s="1"/>
       <c r="D197" s="3"/>
       <c r="E197" s="3"/>
-      <c r="F197" s="4"/>
+      <c r="F197" s="3"/>
       <c r="G197" s="4"/>
       <c r="H197" s="4"/>
       <c r="I197" s="4"/>
-      <c r="J197" s="3"/>
+      <c r="J197" s="4"/>
+      <c r="K197" s="3"/>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="3"/>
@@ -2711,11 +2914,12 @@
       <c r="C198" s="1"/>
       <c r="D198" s="3"/>
       <c r="E198" s="3"/>
-      <c r="F198" s="4"/>
+      <c r="F198" s="3"/>
       <c r="G198" s="4"/>
       <c r="H198" s="4"/>
       <c r="I198" s="4"/>
-      <c r="J198" s="3"/>
+      <c r="J198" s="4"/>
+      <c r="K198" s="3"/>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="3"/>
@@ -2723,11 +2927,12 @@
       <c r="C199" s="1"/>
       <c r="D199" s="3"/>
       <c r="E199" s="3"/>
-      <c r="F199" s="4"/>
+      <c r="F199" s="3"/>
       <c r="G199" s="4"/>
       <c r="H199" s="4"/>
       <c r="I199" s="4"/>
-      <c r="J199" s="3"/>
+      <c r="J199" s="4"/>
+      <c r="K199" s="3"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="3"/>
@@ -2735,11 +2940,12 @@
       <c r="C200" s="1"/>
       <c r="D200" s="3"/>
       <c r="E200" s="3"/>
-      <c r="F200" s="4"/>
+      <c r="F200" s="3"/>
       <c r="G200" s="4"/>
       <c r="H200" s="4"/>
       <c r="I200" s="4"/>
-      <c r="J200" s="3"/>
+      <c r="J200" s="4"/>
+      <c r="K200" s="3"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="3"/>
@@ -2747,11 +2953,12 @@
       <c r="C201" s="1"/>
       <c r="D201" s="3"/>
       <c r="E201" s="3"/>
-      <c r="F201" s="4"/>
+      <c r="F201" s="3"/>
       <c r="G201" s="4"/>
       <c r="H201" s="4"/>
       <c r="I201" s="4"/>
-      <c r="J201" s="3"/>
+      <c r="J201" s="4"/>
+      <c r="K201" s="3"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="3"/>
@@ -2759,11 +2966,12 @@
       <c r="C202" s="1"/>
       <c r="D202" s="3"/>
       <c r="E202" s="3"/>
-      <c r="F202" s="4"/>
+      <c r="F202" s="3"/>
       <c r="G202" s="4"/>
       <c r="H202" s="4"/>
       <c r="I202" s="4"/>
-      <c r="J202" s="3"/>
+      <c r="J202" s="4"/>
+      <c r="K202" s="3"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="3"/>
@@ -2771,11 +2979,12 @@
       <c r="C203" s="1"/>
       <c r="D203" s="3"/>
       <c r="E203" s="3"/>
-      <c r="F203" s="4"/>
+      <c r="F203" s="3"/>
       <c r="G203" s="4"/>
       <c r="H203" s="4"/>
       <c r="I203" s="4"/>
-      <c r="J203" s="3"/>
+      <c r="J203" s="4"/>
+      <c r="K203" s="3"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="3"/>
@@ -2783,11 +2992,12 @@
       <c r="C204" s="1"/>
       <c r="D204" s="3"/>
       <c r="E204" s="3"/>
-      <c r="F204" s="4"/>
+      <c r="F204" s="3"/>
       <c r="G204" s="4"/>
       <c r="H204" s="4"/>
       <c r="I204" s="4"/>
-      <c r="J204" s="3"/>
+      <c r="J204" s="4"/>
+      <c r="K204" s="3"/>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="3"/>
@@ -2795,11 +3005,12 @@
       <c r="C205" s="1"/>
       <c r="D205" s="3"/>
       <c r="E205" s="3"/>
-      <c r="F205" s="4"/>
+      <c r="F205" s="3"/>
       <c r="G205" s="4"/>
       <c r="H205" s="4"/>
       <c r="I205" s="4"/>
-      <c r="J205" s="3"/>
+      <c r="J205" s="4"/>
+      <c r="K205" s="3"/>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="3"/>
@@ -2807,11 +3018,12 @@
       <c r="C206" s="1"/>
       <c r="D206" s="3"/>
       <c r="E206" s="3"/>
-      <c r="F206" s="4"/>
+      <c r="F206" s="3"/>
       <c r="G206" s="4"/>
       <c r="H206" s="4"/>
       <c r="I206" s="4"/>
-      <c r="J206" s="3"/>
+      <c r="J206" s="4"/>
+      <c r="K206" s="3"/>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="3"/>
@@ -2819,11 +3031,12 @@
       <c r="C207" s="1"/>
       <c r="D207" s="3"/>
       <c r="E207" s="3"/>
-      <c r="F207" s="4"/>
+      <c r="F207" s="3"/>
       <c r="G207" s="4"/>
       <c r="H207" s="4"/>
       <c r="I207" s="4"/>
-      <c r="J207" s="3"/>
+      <c r="J207" s="4"/>
+      <c r="K207" s="3"/>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="3"/>
@@ -2831,11 +3044,12 @@
       <c r="C208" s="1"/>
       <c r="D208" s="3"/>
       <c r="E208" s="3"/>
-      <c r="F208" s="4"/>
+      <c r="F208" s="3"/>
       <c r="G208" s="4"/>
       <c r="H208" s="4"/>
       <c r="I208" s="4"/>
-      <c r="J208" s="3"/>
+      <c r="J208" s="4"/>
+      <c r="K208" s="3"/>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="3"/>
@@ -2843,11 +3057,12 @@
       <c r="C209" s="1"/>
       <c r="D209" s="3"/>
       <c r="E209" s="3"/>
-      <c r="F209" s="4"/>
+      <c r="F209" s="3"/>
       <c r="G209" s="4"/>
       <c r="H209" s="4"/>
       <c r="I209" s="4"/>
-      <c r="J209" s="3"/>
+      <c r="J209" s="4"/>
+      <c r="K209" s="3"/>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="3"/>
@@ -2855,11 +3070,12 @@
       <c r="C210" s="1"/>
       <c r="D210" s="3"/>
       <c r="E210" s="3"/>
-      <c r="F210" s="4"/>
+      <c r="F210" s="3"/>
       <c r="G210" s="4"/>
       <c r="H210" s="4"/>
       <c r="I210" s="4"/>
-      <c r="J210" s="3"/>
+      <c r="J210" s="4"/>
+      <c r="K210" s="3"/>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="3"/>
@@ -2867,11 +3083,12 @@
       <c r="C211" s="1"/>
       <c r="D211" s="3"/>
       <c r="E211" s="3"/>
-      <c r="F211" s="4"/>
+      <c r="F211" s="3"/>
       <c r="G211" s="4"/>
       <c r="H211" s="4"/>
       <c r="I211" s="4"/>
-      <c r="J211" s="3"/>
+      <c r="J211" s="4"/>
+      <c r="K211" s="3"/>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="3"/>
@@ -2879,11 +3096,12 @@
       <c r="C212" s="1"/>
       <c r="D212" s="3"/>
       <c r="E212" s="3"/>
-      <c r="F212" s="4"/>
+      <c r="F212" s="3"/>
       <c r="G212" s="4"/>
       <c r="H212" s="4"/>
       <c r="I212" s="4"/>
-      <c r="J212" s="3"/>
+      <c r="J212" s="4"/>
+      <c r="K212" s="3"/>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="3"/>
@@ -2891,11 +3109,12 @@
       <c r="C213" s="1"/>
       <c r="D213" s="3"/>
       <c r="E213" s="3"/>
-      <c r="F213" s="4"/>
+      <c r="F213" s="3"/>
       <c r="G213" s="4"/>
       <c r="H213" s="4"/>
       <c r="I213" s="4"/>
-      <c r="J213" s="3"/>
+      <c r="J213" s="4"/>
+      <c r="K213" s="3"/>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="3"/>
@@ -2903,11 +3122,12 @@
       <c r="C214" s="1"/>
       <c r="D214" s="3"/>
       <c r="E214" s="3"/>
-      <c r="F214" s="4"/>
+      <c r="F214" s="3"/>
       <c r="G214" s="4"/>
       <c r="H214" s="4"/>
       <c r="I214" s="4"/>
-      <c r="J214" s="3"/>
+      <c r="J214" s="4"/>
+      <c r="K214" s="3"/>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="3"/>
@@ -2915,11 +3135,12 @@
       <c r="C215" s="1"/>
       <c r="D215" s="3"/>
       <c r="E215" s="3"/>
-      <c r="F215" s="4"/>
+      <c r="F215" s="3"/>
       <c r="G215" s="4"/>
       <c r="H215" s="4"/>
       <c r="I215" s="4"/>
-      <c r="J215" s="3"/>
+      <c r="J215" s="4"/>
+      <c r="K215" s="3"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="3"/>
@@ -2927,11 +3148,12 @@
       <c r="C216" s="1"/>
       <c r="D216" s="3"/>
       <c r="E216" s="3"/>
-      <c r="F216" s="4"/>
+      <c r="F216" s="3"/>
       <c r="G216" s="4"/>
       <c r="H216" s="4"/>
       <c r="I216" s="4"/>
-      <c r="J216" s="3"/>
+      <c r="J216" s="4"/>
+      <c r="K216" s="3"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="3"/>
@@ -2939,11 +3161,12 @@
       <c r="C217" s="1"/>
       <c r="D217" s="3"/>
       <c r="E217" s="3"/>
-      <c r="F217" s="4"/>
+      <c r="F217" s="3"/>
       <c r="G217" s="4"/>
       <c r="H217" s="4"/>
       <c r="I217" s="4"/>
-      <c r="J217" s="3"/>
+      <c r="J217" s="4"/>
+      <c r="K217" s="3"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="3"/>
@@ -2951,11 +3174,12 @@
       <c r="C218" s="1"/>
       <c r="D218" s="3"/>
       <c r="E218" s="3"/>
-      <c r="F218" s="4"/>
+      <c r="F218" s="3"/>
       <c r="G218" s="4"/>
       <c r="H218" s="4"/>
       <c r="I218" s="4"/>
-      <c r="J218" s="3"/>
+      <c r="J218" s="4"/>
+      <c r="K218" s="3"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="3"/>
@@ -2963,11 +3187,12 @@
       <c r="C219" s="1"/>
       <c r="D219" s="3"/>
       <c r="E219" s="3"/>
-      <c r="F219" s="4"/>
+      <c r="F219" s="3"/>
       <c r="G219" s="4"/>
       <c r="H219" s="4"/>
       <c r="I219" s="4"/>
-      <c r="J219" s="3"/>
+      <c r="J219" s="4"/>
+      <c r="K219" s="3"/>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="3"/>
@@ -2975,11 +3200,12 @@
       <c r="C220" s="1"/>
       <c r="D220" s="3"/>
       <c r="E220" s="3"/>
-      <c r="F220" s="4"/>
+      <c r="F220" s="3"/>
       <c r="G220" s="4"/>
       <c r="H220" s="4"/>
       <c r="I220" s="4"/>
-      <c r="J220" s="3"/>
+      <c r="J220" s="4"/>
+      <c r="K220" s="3"/>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="3"/>
@@ -2987,11 +3213,12 @@
       <c r="C221" s="1"/>
       <c r="D221" s="3"/>
       <c r="E221" s="3"/>
-      <c r="F221" s="4"/>
+      <c r="F221" s="3"/>
       <c r="G221" s="4"/>
       <c r="H221" s="4"/>
       <c r="I221" s="4"/>
-      <c r="J221" s="3"/>
+      <c r="J221" s="4"/>
+      <c r="K221" s="3"/>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="3"/>
@@ -2999,11 +3226,12 @@
       <c r="C222" s="1"/>
       <c r="D222" s="3"/>
       <c r="E222" s="3"/>
-      <c r="F222" s="4"/>
+      <c r="F222" s="3"/>
       <c r="G222" s="4"/>
       <c r="H222" s="4"/>
       <c r="I222" s="4"/>
-      <c r="J222" s="3"/>
+      <c r="J222" s="4"/>
+      <c r="K222" s="3"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="3"/>
@@ -3011,11 +3239,12 @@
       <c r="C223" s="1"/>
       <c r="D223" s="3"/>
       <c r="E223" s="3"/>
-      <c r="F223" s="4"/>
+      <c r="F223" s="3"/>
       <c r="G223" s="4"/>
       <c r="H223" s="4"/>
       <c r="I223" s="4"/>
-      <c r="J223" s="3"/>
+      <c r="J223" s="4"/>
+      <c r="K223" s="3"/>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="3"/>
@@ -3023,11 +3252,12 @@
       <c r="C224" s="1"/>
       <c r="D224" s="3"/>
       <c r="E224" s="3"/>
-      <c r="F224" s="4"/>
+      <c r="F224" s="3"/>
       <c r="G224" s="4"/>
       <c r="H224" s="4"/>
       <c r="I224" s="4"/>
-      <c r="J224" s="3"/>
+      <c r="J224" s="4"/>
+      <c r="K224" s="3"/>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="3"/>
@@ -3035,11 +3265,12 @@
       <c r="C225" s="1"/>
       <c r="D225" s="3"/>
       <c r="E225" s="3"/>
-      <c r="F225" s="4"/>
+      <c r="F225" s="3"/>
       <c r="G225" s="4"/>
       <c r="H225" s="4"/>
       <c r="I225" s="4"/>
-      <c r="J225" s="3"/>
+      <c r="J225" s="4"/>
+      <c r="K225" s="3"/>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="3"/>
@@ -3047,11 +3278,12 @@
       <c r="C226" s="1"/>
       <c r="D226" s="3"/>
       <c r="E226" s="3"/>
-      <c r="F226" s="4"/>
+      <c r="F226" s="3"/>
       <c r="G226" s="4"/>
       <c r="H226" s="4"/>
       <c r="I226" s="4"/>
-      <c r="J226" s="3"/>
+      <c r="J226" s="4"/>
+      <c r="K226" s="3"/>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="3"/>
@@ -3059,11 +3291,12 @@
       <c r="C227" s="1"/>
       <c r="D227" s="3"/>
       <c r="E227" s="3"/>
-      <c r="F227" s="4"/>
+      <c r="F227" s="3"/>
       <c r="G227" s="4"/>
       <c r="H227" s="4"/>
       <c r="I227" s="4"/>
-      <c r="J227" s="3"/>
+      <c r="J227" s="4"/>
+      <c r="K227" s="3"/>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="3"/>
@@ -3071,11 +3304,12 @@
       <c r="C228" s="1"/>
       <c r="D228" s="3"/>
       <c r="E228" s="3"/>
-      <c r="F228" s="4"/>
+      <c r="F228" s="3"/>
       <c r="G228" s="4"/>
       <c r="H228" s="4"/>
       <c r="I228" s="4"/>
-      <c r="J228" s="3"/>
+      <c r="J228" s="4"/>
+      <c r="K228" s="3"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="3"/>
@@ -3083,11 +3317,12 @@
       <c r="C229" s="1"/>
       <c r="D229" s="3"/>
       <c r="E229" s="3"/>
-      <c r="F229" s="4"/>
+      <c r="F229" s="3"/>
       <c r="G229" s="4"/>
       <c r="H229" s="4"/>
       <c r="I229" s="4"/>
-      <c r="J229" s="3"/>
+      <c r="J229" s="4"/>
+      <c r="K229" s="3"/>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="3"/>
@@ -3095,11 +3330,12 @@
       <c r="C230" s="1"/>
       <c r="D230" s="3"/>
       <c r="E230" s="3"/>
-      <c r="F230" s="4"/>
+      <c r="F230" s="3"/>
       <c r="G230" s="4"/>
       <c r="H230" s="4"/>
       <c r="I230" s="4"/>
-      <c r="J230" s="3"/>
+      <c r="J230" s="4"/>
+      <c r="K230" s="3"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="3"/>
@@ -3107,11 +3343,12 @@
       <c r="C231" s="1"/>
       <c r="D231" s="3"/>
       <c r="E231" s="3"/>
-      <c r="F231" s="4"/>
+      <c r="F231" s="3"/>
       <c r="G231" s="4"/>
       <c r="H231" s="4"/>
       <c r="I231" s="4"/>
-      <c r="J231" s="3"/>
+      <c r="J231" s="4"/>
+      <c r="K231" s="3"/>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="3"/>
@@ -3119,11 +3356,12 @@
       <c r="C232" s="1"/>
       <c r="D232" s="3"/>
       <c r="E232" s="3"/>
-      <c r="F232" s="4"/>
+      <c r="F232" s="3"/>
       <c r="G232" s="4"/>
       <c r="H232" s="4"/>
       <c r="I232" s="4"/>
-      <c r="J232" s="3"/>
+      <c r="J232" s="4"/>
+      <c r="K232" s="3"/>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="3"/>
@@ -3131,11 +3369,12 @@
       <c r="C233" s="1"/>
       <c r="D233" s="3"/>
       <c r="E233" s="3"/>
-      <c r="F233" s="4"/>
+      <c r="F233" s="3"/>
       <c r="G233" s="4"/>
       <c r="H233" s="4"/>
       <c r="I233" s="4"/>
-      <c r="J233" s="3"/>
+      <c r="J233" s="4"/>
+      <c r="K233" s="3"/>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="3"/>
@@ -3143,11 +3382,12 @@
       <c r="C234" s="1"/>
       <c r="D234" s="3"/>
       <c r="E234" s="3"/>
-      <c r="F234" s="4"/>
+      <c r="F234" s="3"/>
       <c r="G234" s="4"/>
       <c r="H234" s="4"/>
       <c r="I234" s="4"/>
-      <c r="J234" s="3"/>
+      <c r="J234" s="4"/>
+      <c r="K234" s="3"/>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="3"/>
@@ -3155,11 +3395,12 @@
       <c r="C235" s="1"/>
       <c r="D235" s="3"/>
       <c r="E235" s="3"/>
-      <c r="F235" s="4"/>
+      <c r="F235" s="3"/>
       <c r="G235" s="4"/>
       <c r="H235" s="4"/>
       <c r="I235" s="4"/>
-      <c r="J235" s="3"/>
+      <c r="J235" s="4"/>
+      <c r="K235" s="3"/>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="3"/>
@@ -3167,11 +3408,12 @@
       <c r="C236" s="1"/>
       <c r="D236" s="3"/>
       <c r="E236" s="3"/>
-      <c r="F236" s="4"/>
+      <c r="F236" s="3"/>
       <c r="G236" s="4"/>
       <c r="H236" s="4"/>
       <c r="I236" s="4"/>
-      <c r="J236" s="3"/>
+      <c r="J236" s="4"/>
+      <c r="K236" s="3"/>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="3"/>
@@ -3179,11 +3421,12 @@
       <c r="C237" s="1"/>
       <c r="D237" s="3"/>
       <c r="E237" s="3"/>
-      <c r="F237" s="4"/>
+      <c r="F237" s="3"/>
       <c r="G237" s="4"/>
       <c r="H237" s="4"/>
       <c r="I237" s="4"/>
-      <c r="J237" s="3"/>
+      <c r="J237" s="4"/>
+      <c r="K237" s="3"/>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="3"/>
@@ -3191,11 +3434,12 @@
       <c r="C238" s="1"/>
       <c r="D238" s="3"/>
       <c r="E238" s="3"/>
-      <c r="F238" s="4"/>
+      <c r="F238" s="3"/>
       <c r="G238" s="4"/>
       <c r="H238" s="4"/>
       <c r="I238" s="4"/>
-      <c r="J238" s="3"/>
+      <c r="J238" s="4"/>
+      <c r="K238" s="3"/>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="3"/>
@@ -3203,11 +3447,12 @@
       <c r="C239" s="1"/>
       <c r="D239" s="3"/>
       <c r="E239" s="3"/>
-      <c r="F239" s="4"/>
+      <c r="F239" s="3"/>
       <c r="G239" s="4"/>
       <c r="H239" s="4"/>
       <c r="I239" s="4"/>
-      <c r="J239" s="3"/>
+      <c r="J239" s="4"/>
+      <c r="K239" s="3"/>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="3"/>
@@ -3215,11 +3460,12 @@
       <c r="C240" s="1"/>
       <c r="D240" s="3"/>
       <c r="E240" s="3"/>
-      <c r="F240" s="4"/>
+      <c r="F240" s="3"/>
       <c r="G240" s="4"/>
       <c r="H240" s="4"/>
       <c r="I240" s="4"/>
-      <c r="J240" s="3"/>
+      <c r="J240" s="4"/>
+      <c r="K240" s="3"/>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="3"/>
@@ -3227,11 +3473,12 @@
       <c r="C241" s="1"/>
       <c r="D241" s="3"/>
       <c r="E241" s="3"/>
-      <c r="F241" s="4"/>
+      <c r="F241" s="3"/>
       <c r="G241" s="4"/>
       <c r="H241" s="4"/>
       <c r="I241" s="4"/>
-      <c r="J241" s="3"/>
+      <c r="J241" s="4"/>
+      <c r="K241" s="3"/>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="3"/>
@@ -3239,11 +3486,12 @@
       <c r="C242" s="1"/>
       <c r="D242" s="3"/>
       <c r="E242" s="3"/>
-      <c r="F242" s="4"/>
+      <c r="F242" s="3"/>
       <c r="G242" s="4"/>
       <c r="H242" s="4"/>
       <c r="I242" s="4"/>
-      <c r="J242" s="3"/>
+      <c r="J242" s="4"/>
+      <c r="K242" s="3"/>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="3"/>
@@ -3251,11 +3499,12 @@
       <c r="C243" s="1"/>
       <c r="D243" s="3"/>
       <c r="E243" s="3"/>
-      <c r="F243" s="4"/>
+      <c r="F243" s="3"/>
       <c r="G243" s="4"/>
       <c r="H243" s="4"/>
       <c r="I243" s="4"/>
-      <c r="J243" s="3"/>
+      <c r="J243" s="4"/>
+      <c r="K243" s="3"/>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="3"/>
@@ -3426,7 +3675,7 @@
       <c r="B299" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:J243"/>
+  <autoFilter ref="B1:K243"/>
   <dataValidations count="5">
     <dataValidation allowBlank="false" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A243" type="list">
       <formula1>"Bilgisayar Teknolojileri,Elektrik ve Enerji,Muhasebe ve Vergi Uygulamaları,Yönetim ve Organizasyon,Finans - Bankacılık ve Sigortacılık,El Sanatları,Seyahat - Turizm ve Eğlence Hizmetleri,Ulaştırma Hizmetleri,Mimarlık Ve Şehir Planlama"</formula1>
@@ -3436,7 +3685,7 @@
       <formula1>"Zorunlu,Seçmeli,Üniversite Seçmeli,Staj"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J1001" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2:K1001" type="list">
       <formula1>"Derslik,Bilgisayar Laboratuvarı,Uzaktan Eğitim Sınıfı,Karma"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3453,8 +3702,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Sayfa &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ders listesine grupno eklendi
</commit_message>
<xml_diff>
--- a/Public/assets/downloads/Ders Listesi.xlsx
+++ b/Public/assets/downloads/Ders Listesi.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sayfa1!$B$1:$J$243</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sayfa1!$B$1:$K$243</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
   <si>
     <t xml:space="preserve">Bölüm </t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dersin Kodu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grup No</t>
   </si>
   <si>
     <t xml:space="preserve">Dersin Adı</t>
@@ -367,7 +370,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -389,10 +392,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,12 +539,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J299"/>
+  <dimension ref="A1:K299"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -553,10 +552,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="48.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="34.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="48.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="34.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -589,6 +589,9 @@
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,11 +600,14 @@
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="3"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
@@ -609,11 +615,12 @@
       <c r="C3" s="1"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="3"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3"/>
@@ -621,11 +628,12 @@
       <c r="C4" s="1"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
@@ -633,11 +641,12 @@
       <c r="C5" s="1"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
@@ -645,11 +654,12 @@
       <c r="C6" s="1"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3"/>
@@ -657,11 +667,12 @@
       <c r="C7" s="1"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3"/>
@@ -669,11 +680,12 @@
       <c r="C8" s="1"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
@@ -681,11 +693,12 @@
       <c r="C9" s="1"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="3"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
@@ -693,11 +706,12 @@
       <c r="C10" s="1"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
@@ -705,11 +719,12 @@
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="3"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
@@ -717,11 +732,12 @@
       <c r="C12" s="1"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3"/>
@@ -729,11 +745,12 @@
       <c r="C13" s="1"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
@@ -741,11 +758,12 @@
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
@@ -753,11 +771,12 @@
       <c r="C15" s="1"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="3"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3"/>
@@ -765,11 +784,12 @@
       <c r="C16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="3"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3"/>
@@ -777,11 +797,12 @@
       <c r="C17" s="1"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="3"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3"/>
@@ -789,11 +810,12 @@
       <c r="C18" s="1"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="3"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3"/>
@@ -801,11 +823,12 @@
       <c r="C19" s="1"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="3"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="3"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
@@ -813,11 +836,12 @@
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="3"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
@@ -825,11 +849,12 @@
       <c r="C21" s="1"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="3"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="3"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>
@@ -837,11 +862,12 @@
       <c r="C22" s="1"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="4"/>
+      <c r="F22" s="3"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3"/>
@@ -849,11 +875,12 @@
       <c r="C23" s="1"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="3"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="3"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
@@ -861,11 +888,12 @@
       <c r="C24" s="1"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="4"/>
+      <c r="F24" s="3"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3"/>
@@ -873,11 +901,12 @@
       <c r="C25" s="1"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="4"/>
+      <c r="F25" s="3"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="3"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
@@ -885,11 +914,12 @@
       <c r="C26" s="1"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="3"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3"/>
@@ -897,11 +927,12 @@
       <c r="C27" s="1"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="4"/>
+      <c r="F27" s="3"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="3"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
@@ -909,11 +940,12 @@
       <c r="C28" s="1"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="3"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="3"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
@@ -921,11 +953,12 @@
       <c r="C29" s="1"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="4"/>
+      <c r="F29" s="3"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="3"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
@@ -933,11 +966,12 @@
       <c r="C30" s="1"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="4"/>
+      <c r="F30" s="3"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="3"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
@@ -945,11 +979,12 @@
       <c r="C31" s="1"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="4"/>
+      <c r="F31" s="3"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="3"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
@@ -957,11 +992,12 @@
       <c r="C32" s="1"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="4"/>
+      <c r="F32" s="3"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="3"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3"/>
@@ -969,11 +1005,12 @@
       <c r="C33" s="1"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="4"/>
+      <c r="F33" s="3"/>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="3"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
@@ -981,11 +1018,12 @@
       <c r="C34" s="1"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="4"/>
+      <c r="F34" s="3"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="3"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3"/>
@@ -993,11 +1031,12 @@
       <c r="C35" s="1"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="4"/>
+      <c r="F35" s="3"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="3"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
@@ -1005,11 +1044,12 @@
       <c r="C36" s="1"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="4"/>
+      <c r="F36" s="3"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="3"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3"/>
@@ -1021,7 +1061,8 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="3"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3"/>
@@ -1033,7 +1074,8 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
       <c r="I38" s="4"/>
-      <c r="J38" s="3"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3"/>
@@ -1045,7 +1087,8 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="3"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3"/>
@@ -1057,7 +1100,8 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
-      <c r="J40" s="3"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3"/>
@@ -1069,7 +1113,8 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="3"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3"/>
@@ -1081,7 +1126,8 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
-      <c r="J42" s="3"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3"/>
@@ -1093,7 +1139,8 @@
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="3"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3"/>
@@ -1105,7 +1152,8 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
-      <c r="J44" s="3"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3"/>
@@ -1117,7 +1165,8 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="3"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3"/>
@@ -1129,7 +1178,8 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
       <c r="I46" s="4"/>
-      <c r="J46" s="3"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3"/>
@@ -1141,7 +1191,8 @@
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="3"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3"/>
@@ -1153,7 +1204,8 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="3"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3"/>
@@ -1165,7 +1217,8 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="3"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3"/>
@@ -1177,7 +1230,8 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
-      <c r="J50" s="3"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3"/>
@@ -1189,7 +1243,8 @@
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
-      <c r="J51" s="3"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3"/>
@@ -1201,7 +1256,8 @@
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
-      <c r="J52" s="3"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3"/>
@@ -1213,7 +1269,8 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
-      <c r="J53" s="3"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3"/>
@@ -1225,7 +1282,8 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
-      <c r="J54" s="3"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="3"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3"/>
@@ -1237,7 +1295,8 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
-      <c r="J55" s="3"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="3"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3"/>
@@ -1249,7 +1308,8 @@
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
-      <c r="J56" s="3"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="3"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3"/>
@@ -1261,7 +1321,8 @@
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
-      <c r="J57" s="3"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="3"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
@@ -1273,7 +1334,8 @@
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
-      <c r="J58" s="3"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="3"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
@@ -1285,7 +1347,8 @@
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
-      <c r="J59" s="3"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3"/>
@@ -1293,11 +1356,12 @@
       <c r="C60" s="1"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="4"/>
+      <c r="F60" s="3"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
-      <c r="J60" s="3"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="3"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3"/>
@@ -1305,11 +1369,12 @@
       <c r="C61" s="1"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
+      <c r="F61" s="3"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
-      <c r="J61" s="3"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="3"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3"/>
@@ -1317,11 +1382,12 @@
       <c r="C62" s="1"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="4"/>
+      <c r="F62" s="3"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
-      <c r="J62" s="3"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="3"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3"/>
@@ -1329,11 +1395,12 @@
       <c r="C63" s="1"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
+      <c r="F63" s="3"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
-      <c r="J63" s="3"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="3"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3"/>
@@ -1341,11 +1408,12 @@
       <c r="C64" s="1"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="4"/>
+      <c r="F64" s="3"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
-      <c r="J64" s="3"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="3"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3"/>
@@ -1353,11 +1421,12 @@
       <c r="C65" s="1"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="4"/>
+      <c r="F65" s="3"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="3"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3"/>
@@ -1365,11 +1434,12 @@
       <c r="C66" s="1"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="4"/>
+      <c r="F66" s="3"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
-      <c r="J66" s="3"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="3"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3"/>
@@ -1377,11 +1447,12 @@
       <c r="C67" s="1"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
-      <c r="F67" s="4"/>
+      <c r="F67" s="3"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
-      <c r="J67" s="3"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="3"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3"/>
@@ -1389,11 +1460,12 @@
       <c r="C68" s="1"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
-      <c r="F68" s="4"/>
+      <c r="F68" s="3"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
-      <c r="J68" s="3"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="3"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3"/>
@@ -1401,11 +1473,12 @@
       <c r="C69" s="1"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
-      <c r="F69" s="4"/>
+      <c r="F69" s="3"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
-      <c r="J69" s="3"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="3"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3"/>
@@ -1413,11 +1486,12 @@
       <c r="C70" s="1"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
-      <c r="F70" s="4"/>
+      <c r="F70" s="3"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
-      <c r="J70" s="3"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="3"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3"/>
@@ -1425,11 +1499,12 @@
       <c r="C71" s="1"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
-      <c r="F71" s="4"/>
+      <c r="F71" s="3"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
-      <c r="J71" s="3"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="3"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3"/>
@@ -1437,11 +1512,12 @@
       <c r="C72" s="1"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
-      <c r="F72" s="4"/>
+      <c r="F72" s="3"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
-      <c r="J72" s="3"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="3"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3"/>
@@ -1449,11 +1525,12 @@
       <c r="C73" s="1"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
-      <c r="F73" s="4"/>
+      <c r="F73" s="3"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
-      <c r="J73" s="3"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="3"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3"/>
@@ -1461,11 +1538,12 @@
       <c r="C74" s="1"/>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
-      <c r="F74" s="4"/>
+      <c r="F74" s="3"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
-      <c r="J74" s="3"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="3"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3"/>
@@ -1473,11 +1551,12 @@
       <c r="C75" s="1"/>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
-      <c r="F75" s="4"/>
+      <c r="F75" s="3"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
-      <c r="J75" s="3"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="3"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3"/>
@@ -1485,11 +1564,12 @@
       <c r="C76" s="1"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
-      <c r="F76" s="4"/>
+      <c r="F76" s="3"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
-      <c r="J76" s="3"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3"/>
@@ -1497,11 +1577,12 @@
       <c r="C77" s="1"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
-      <c r="F77" s="4"/>
+      <c r="F77" s="3"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
-      <c r="J77" s="3"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="3"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3"/>
@@ -1509,11 +1590,12 @@
       <c r="C78" s="1"/>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="4"/>
+      <c r="F78" s="3"/>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
-      <c r="J78" s="3"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="3"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3"/>
@@ -1521,11 +1603,12 @@
       <c r="C79" s="1"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="4"/>
+      <c r="F79" s="3"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
-      <c r="J79" s="3"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="3"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3"/>
@@ -1533,11 +1616,12 @@
       <c r="C80" s="1"/>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="4"/>
+      <c r="F80" s="3"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
-      <c r="J80" s="3"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="3"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3"/>
@@ -1545,11 +1629,12 @@
       <c r="C81" s="1"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="4"/>
+      <c r="F81" s="3"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
-      <c r="J81" s="3"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="3"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3"/>
@@ -1557,11 +1642,12 @@
       <c r="C82" s="1"/>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="4"/>
+      <c r="F82" s="3"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
-      <c r="J82" s="3"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3"/>
@@ -1569,11 +1655,12 @@
       <c r="C83" s="1"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="4"/>
+      <c r="F83" s="3"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
-      <c r="J83" s="3"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3"/>
@@ -1581,11 +1668,12 @@
       <c r="C84" s="1"/>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="4"/>
+      <c r="F84" s="3"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
-      <c r="J84" s="3"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="3"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3"/>
@@ -1593,11 +1681,12 @@
       <c r="C85" s="1"/>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="4"/>
+      <c r="F85" s="3"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
-      <c r="J85" s="3"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="3"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3"/>
@@ -1605,11 +1694,12 @@
       <c r="C86" s="1"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
-      <c r="F86" s="4"/>
+      <c r="F86" s="3"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
-      <c r="J86" s="3"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="3"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3"/>
@@ -1617,11 +1707,12 @@
       <c r="C87" s="1"/>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
-      <c r="F87" s="4"/>
+      <c r="F87" s="3"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
-      <c r="J87" s="3"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="3"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3"/>
@@ -1629,11 +1720,12 @@
       <c r="C88" s="1"/>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
-      <c r="F88" s="4"/>
+      <c r="F88" s="3"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
-      <c r="J88" s="3"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="3"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3"/>
@@ -1641,11 +1733,12 @@
       <c r="C89" s="1"/>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
-      <c r="F89" s="4"/>
+      <c r="F89" s="3"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
-      <c r="J89" s="3"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="3"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3"/>
@@ -1653,11 +1746,12 @@
       <c r="C90" s="1"/>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
-      <c r="F90" s="4"/>
+      <c r="F90" s="3"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
-      <c r="J90" s="3"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="3"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3"/>
@@ -1665,11 +1759,12 @@
       <c r="C91" s="1"/>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
-      <c r="F91" s="4"/>
+      <c r="F91" s="3"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
-      <c r="J91" s="3"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="3"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3"/>
@@ -1677,11 +1772,12 @@
       <c r="C92" s="1"/>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
-      <c r="F92" s="4"/>
+      <c r="F92" s="3"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
-      <c r="J92" s="3"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="3"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3"/>
@@ -1689,11 +1785,12 @@
       <c r="C93" s="1"/>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
-      <c r="F93" s="4"/>
+      <c r="F93" s="3"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
-      <c r="J93" s="3"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="3"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3"/>
@@ -1701,11 +1798,12 @@
       <c r="C94" s="1"/>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
-      <c r="F94" s="4"/>
+      <c r="F94" s="3"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
-      <c r="J94" s="3"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="3"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3"/>
@@ -1713,11 +1811,12 @@
       <c r="C95" s="1"/>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
-      <c r="F95" s="4"/>
+      <c r="F95" s="3"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
-      <c r="J95" s="3"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="3"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3"/>
@@ -1725,11 +1824,12 @@
       <c r="C96" s="1"/>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
-      <c r="F96" s="4"/>
+      <c r="F96" s="3"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
-      <c r="J96" s="3"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="3"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3"/>
@@ -1737,11 +1837,12 @@
       <c r="C97" s="1"/>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
-      <c r="F97" s="4"/>
+      <c r="F97" s="3"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
-      <c r="J97" s="3"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3"/>
@@ -1749,11 +1850,12 @@
       <c r="C98" s="1"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
-      <c r="F98" s="4"/>
+      <c r="F98" s="3"/>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
-      <c r="J98" s="3"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="3"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3"/>
@@ -1761,11 +1863,12 @@
       <c r="C99" s="1"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
-      <c r="F99" s="4"/>
+      <c r="F99" s="3"/>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
-      <c r="J99" s="3"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="3"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3"/>
@@ -1773,11 +1876,12 @@
       <c r="C100" s="1"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
-      <c r="F100" s="4"/>
+      <c r="F100" s="3"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
-      <c r="J100" s="3"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="3"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3"/>
@@ -1785,11 +1889,12 @@
       <c r="C101" s="1"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
-      <c r="F101" s="4"/>
+      <c r="F101" s="3"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
-      <c r="J101" s="3"/>
+      <c r="J101" s="4"/>
+      <c r="K101" s="3"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3"/>
@@ -1797,11 +1902,12 @@
       <c r="C102" s="1"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
-      <c r="F102" s="4"/>
+      <c r="F102" s="3"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
-      <c r="J102" s="3"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="3"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3"/>
@@ -1809,11 +1915,12 @@
       <c r="C103" s="1"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
-      <c r="F103" s="4"/>
+      <c r="F103" s="3"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
-      <c r="J103" s="3"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="3"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3"/>
@@ -1821,11 +1928,12 @@
       <c r="C104" s="1"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
-      <c r="F104" s="4"/>
+      <c r="F104" s="3"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
-      <c r="J104" s="3"/>
+      <c r="J104" s="4"/>
+      <c r="K104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3"/>
@@ -1833,11 +1941,12 @@
       <c r="C105" s="1"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
-      <c r="F105" s="4"/>
+      <c r="F105" s="3"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
-      <c r="J105" s="3"/>
+      <c r="J105" s="4"/>
+      <c r="K105" s="3"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3"/>
@@ -1845,11 +1954,12 @@
       <c r="C106" s="1"/>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
-      <c r="F106" s="4"/>
+      <c r="F106" s="3"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
-      <c r="J106" s="3"/>
+      <c r="J106" s="4"/>
+      <c r="K106" s="3"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3"/>
@@ -1857,11 +1967,12 @@
       <c r="C107" s="1"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
-      <c r="F107" s="4"/>
+      <c r="F107" s="3"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
-      <c r="J107" s="3"/>
+      <c r="J107" s="4"/>
+      <c r="K107" s="3"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3"/>
@@ -1869,11 +1980,12 @@
       <c r="C108" s="1"/>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
-      <c r="F108" s="4"/>
+      <c r="F108" s="3"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
-      <c r="J108" s="3"/>
+      <c r="J108" s="4"/>
+      <c r="K108" s="3"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3"/>
@@ -1881,11 +1993,12 @@
       <c r="C109" s="1"/>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
-      <c r="F109" s="4"/>
+      <c r="F109" s="3"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
-      <c r="J109" s="3"/>
+      <c r="J109" s="4"/>
+      <c r="K109" s="3"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3"/>
@@ -1893,11 +2006,12 @@
       <c r="C110" s="1"/>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
-      <c r="F110" s="4"/>
+      <c r="F110" s="3"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
-      <c r="J110" s="3"/>
+      <c r="J110" s="4"/>
+      <c r="K110" s="3"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3"/>
@@ -1905,11 +2019,12 @@
       <c r="C111" s="1"/>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
-      <c r="F111" s="4"/>
+      <c r="F111" s="3"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
-      <c r="J111" s="3"/>
+      <c r="J111" s="4"/>
+      <c r="K111" s="3"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3"/>
@@ -1917,11 +2032,12 @@
       <c r="C112" s="1"/>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
-      <c r="F112" s="4"/>
+      <c r="F112" s="3"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
-      <c r="J112" s="3"/>
+      <c r="J112" s="4"/>
+      <c r="K112" s="3"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3"/>
@@ -1929,11 +2045,12 @@
       <c r="C113" s="1"/>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
-      <c r="F113" s="4"/>
+      <c r="F113" s="3"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
       <c r="I113" s="4"/>
-      <c r="J113" s="3"/>
+      <c r="J113" s="4"/>
+      <c r="K113" s="3"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3"/>
@@ -1941,11 +2058,12 @@
       <c r="C114" s="1"/>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
-      <c r="F114" s="4"/>
+      <c r="F114" s="3"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
-      <c r="J114" s="3"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="3"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3"/>
@@ -1953,11 +2071,12 @@
       <c r="C115" s="1"/>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
-      <c r="F115" s="4"/>
+      <c r="F115" s="3"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
-      <c r="J115" s="3"/>
+      <c r="J115" s="4"/>
+      <c r="K115" s="3"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3"/>
@@ -1965,11 +2084,12 @@
       <c r="C116" s="1"/>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
-      <c r="F116" s="4"/>
+      <c r="F116" s="3"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
-      <c r="J116" s="3"/>
+      <c r="J116" s="4"/>
+      <c r="K116" s="3"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3"/>
@@ -1977,11 +2097,12 @@
       <c r="C117" s="1"/>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
-      <c r="F117" s="4"/>
+      <c r="F117" s="3"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
-      <c r="J117" s="3"/>
+      <c r="J117" s="4"/>
+      <c r="K117" s="3"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3"/>
@@ -1989,11 +2110,12 @@
       <c r="C118" s="1"/>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
-      <c r="F118" s="4"/>
+      <c r="F118" s="3"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
-      <c r="J118" s="3"/>
+      <c r="J118" s="4"/>
+      <c r="K118" s="3"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3"/>
@@ -2001,11 +2123,12 @@
       <c r="C119" s="1"/>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
-      <c r="F119" s="4"/>
+      <c r="F119" s="3"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
-      <c r="J119" s="3"/>
+      <c r="J119" s="4"/>
+      <c r="K119" s="3"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3"/>
@@ -2013,11 +2136,12 @@
       <c r="C120" s="1"/>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
-      <c r="F120" s="4"/>
+      <c r="F120" s="3"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
-      <c r="J120" s="3"/>
+      <c r="J120" s="4"/>
+      <c r="K120" s="3"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3"/>
@@ -2025,11 +2149,12 @@
       <c r="C121" s="1"/>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
-      <c r="F121" s="4"/>
+      <c r="F121" s="3"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
-      <c r="J121" s="3"/>
+      <c r="J121" s="4"/>
+      <c r="K121" s="3"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3"/>
@@ -2037,11 +2162,12 @@
       <c r="C122" s="1"/>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
-      <c r="F122" s="4"/>
+      <c r="F122" s="3"/>
       <c r="G122" s="4"/>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
-      <c r="J122" s="3"/>
+      <c r="J122" s="4"/>
+      <c r="K122" s="3"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3"/>
@@ -2049,11 +2175,12 @@
       <c r="C123" s="1"/>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
-      <c r="F123" s="4"/>
+      <c r="F123" s="3"/>
       <c r="G123" s="4"/>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
-      <c r="J123" s="3"/>
+      <c r="J123" s="4"/>
+      <c r="K123" s="3"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3"/>
@@ -2061,11 +2188,12 @@
       <c r="C124" s="1"/>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
-      <c r="F124" s="4"/>
+      <c r="F124" s="3"/>
       <c r="G124" s="4"/>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
-      <c r="J124" s="3"/>
+      <c r="J124" s="4"/>
+      <c r="K124" s="3"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3"/>
@@ -2073,11 +2201,12 @@
       <c r="C125" s="1"/>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
-      <c r="F125" s="4"/>
+      <c r="F125" s="3"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
-      <c r="J125" s="3"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="3"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3"/>
@@ -2085,11 +2214,12 @@
       <c r="C126" s="1"/>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
-      <c r="F126" s="4"/>
+      <c r="F126" s="3"/>
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
-      <c r="J126" s="3"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="3"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3"/>
@@ -2097,11 +2227,12 @@
       <c r="C127" s="1"/>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
-      <c r="F127" s="4"/>
+      <c r="F127" s="3"/>
       <c r="G127" s="4"/>
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
-      <c r="J127" s="3"/>
+      <c r="J127" s="4"/>
+      <c r="K127" s="3"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3"/>
@@ -2109,11 +2240,12 @@
       <c r="C128" s="1"/>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
-      <c r="F128" s="4"/>
+      <c r="F128" s="3"/>
       <c r="G128" s="4"/>
       <c r="H128" s="4"/>
       <c r="I128" s="4"/>
-      <c r="J128" s="3"/>
+      <c r="J128" s="4"/>
+      <c r="K128" s="3"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3"/>
@@ -2121,11 +2253,12 @@
       <c r="C129" s="1"/>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
-      <c r="F129" s="4"/>
+      <c r="F129" s="3"/>
       <c r="G129" s="4"/>
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
-      <c r="J129" s="3"/>
+      <c r="J129" s="4"/>
+      <c r="K129" s="3"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3"/>
@@ -2133,11 +2266,12 @@
       <c r="C130" s="1"/>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
-      <c r="F130" s="4"/>
+      <c r="F130" s="3"/>
       <c r="G130" s="4"/>
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
-      <c r="J130" s="3"/>
+      <c r="J130" s="4"/>
+      <c r="K130" s="3"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="3"/>
@@ -2145,11 +2279,12 @@
       <c r="C131" s="1"/>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
-      <c r="F131" s="4"/>
+      <c r="F131" s="3"/>
       <c r="G131" s="4"/>
       <c r="H131" s="4"/>
       <c r="I131" s="4"/>
-      <c r="J131" s="3"/>
+      <c r="J131" s="4"/>
+      <c r="K131" s="3"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3"/>
@@ -2157,11 +2292,12 @@
       <c r="C132" s="1"/>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
-      <c r="F132" s="4"/>
+      <c r="F132" s="3"/>
       <c r="G132" s="4"/>
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
-      <c r="J132" s="3"/>
+      <c r="J132" s="4"/>
+      <c r="K132" s="3"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3"/>
@@ -2169,11 +2305,12 @@
       <c r="C133" s="1"/>
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
-      <c r="F133" s="4"/>
+      <c r="F133" s="3"/>
       <c r="G133" s="4"/>
       <c r="H133" s="4"/>
       <c r="I133" s="4"/>
-      <c r="J133" s="3"/>
+      <c r="J133" s="4"/>
+      <c r="K133" s="3"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3"/>
@@ -2181,11 +2318,12 @@
       <c r="C134" s="1"/>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
-      <c r="F134" s="4"/>
+      <c r="F134" s="3"/>
       <c r="G134" s="4"/>
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
-      <c r="J134" s="3"/>
+      <c r="J134" s="4"/>
+      <c r="K134" s="3"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3"/>
@@ -2193,11 +2331,12 @@
       <c r="C135" s="1"/>
       <c r="D135" s="3"/>
       <c r="E135" s="3"/>
-      <c r="F135" s="4"/>
+      <c r="F135" s="3"/>
       <c r="G135" s="4"/>
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
-      <c r="J135" s="3"/>
+      <c r="J135" s="4"/>
+      <c r="K135" s="3"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3"/>
@@ -2205,11 +2344,12 @@
       <c r="C136" s="1"/>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
-      <c r="F136" s="4"/>
+      <c r="F136" s="3"/>
       <c r="G136" s="4"/>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
-      <c r="J136" s="3"/>
+      <c r="J136" s="4"/>
+      <c r="K136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3"/>
@@ -2217,11 +2357,12 @@
       <c r="C137" s="1"/>
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>
-      <c r="F137" s="4"/>
+      <c r="F137" s="3"/>
       <c r="G137" s="4"/>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
-      <c r="J137" s="3"/>
+      <c r="J137" s="4"/>
+      <c r="K137" s="3"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3"/>
@@ -2229,11 +2370,12 @@
       <c r="C138" s="1"/>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
-      <c r="F138" s="4"/>
+      <c r="F138" s="3"/>
       <c r="G138" s="4"/>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
-      <c r="J138" s="3"/>
+      <c r="J138" s="4"/>
+      <c r="K138" s="3"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3"/>
@@ -2241,11 +2383,12 @@
       <c r="C139" s="1"/>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
-      <c r="F139" s="4"/>
+      <c r="F139" s="3"/>
       <c r="G139" s="4"/>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
-      <c r="J139" s="3"/>
+      <c r="J139" s="4"/>
+      <c r="K139" s="3"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3"/>
@@ -2253,11 +2396,12 @@
       <c r="C140" s="1"/>
       <c r="D140" s="3"/>
       <c r="E140" s="3"/>
-      <c r="F140" s="4"/>
+      <c r="F140" s="3"/>
       <c r="G140" s="4"/>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
-      <c r="J140" s="3"/>
+      <c r="J140" s="4"/>
+      <c r="K140" s="3"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3"/>
@@ -2265,11 +2409,12 @@
       <c r="C141" s="1"/>
       <c r="D141" s="3"/>
       <c r="E141" s="3"/>
-      <c r="F141" s="4"/>
+      <c r="F141" s="3"/>
       <c r="G141" s="4"/>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
-      <c r="J141" s="3"/>
+      <c r="J141" s="4"/>
+      <c r="K141" s="3"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3"/>
@@ -2277,11 +2422,12 @@
       <c r="C142" s="1"/>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
-      <c r="F142" s="4"/>
+      <c r="F142" s="3"/>
       <c r="G142" s="4"/>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
-      <c r="J142" s="3"/>
+      <c r="J142" s="4"/>
+      <c r="K142" s="3"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3"/>
@@ -2289,11 +2435,12 @@
       <c r="C143" s="1"/>
       <c r="D143" s="3"/>
       <c r="E143" s="3"/>
-      <c r="F143" s="4"/>
+      <c r="F143" s="3"/>
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
-      <c r="J143" s="3"/>
+      <c r="J143" s="4"/>
+      <c r="K143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3"/>
@@ -2301,11 +2448,12 @@
       <c r="C144" s="1"/>
       <c r="D144" s="3"/>
       <c r="E144" s="3"/>
-      <c r="F144" s="4"/>
+      <c r="F144" s="3"/>
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
-      <c r="J144" s="3"/>
+      <c r="J144" s="4"/>
+      <c r="K144" s="3"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3"/>
@@ -2313,11 +2461,12 @@
       <c r="C145" s="1"/>
       <c r="D145" s="3"/>
       <c r="E145" s="3"/>
-      <c r="F145" s="4"/>
+      <c r="F145" s="3"/>
       <c r="G145" s="4"/>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
-      <c r="J145" s="3"/>
+      <c r="J145" s="4"/>
+      <c r="K145" s="3"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="3"/>
@@ -2325,11 +2474,12 @@
       <c r="C146" s="1"/>
       <c r="D146" s="3"/>
       <c r="E146" s="3"/>
-      <c r="F146" s="4"/>
+      <c r="F146" s="3"/>
       <c r="G146" s="4"/>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
-      <c r="J146" s="3"/>
+      <c r="J146" s="4"/>
+      <c r="K146" s="3"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3"/>
@@ -2337,11 +2487,12 @@
       <c r="C147" s="1"/>
       <c r="D147" s="3"/>
       <c r="E147" s="3"/>
-      <c r="F147" s="4"/>
+      <c r="F147" s="3"/>
       <c r="G147" s="4"/>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
-      <c r="J147" s="3"/>
+      <c r="J147" s="4"/>
+      <c r="K147" s="3"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3"/>
@@ -2349,11 +2500,12 @@
       <c r="C148" s="1"/>
       <c r="D148" s="3"/>
       <c r="E148" s="3"/>
-      <c r="F148" s="4"/>
+      <c r="F148" s="3"/>
       <c r="G148" s="4"/>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
-      <c r="J148" s="3"/>
+      <c r="J148" s="4"/>
+      <c r="K148" s="3"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3"/>
@@ -2361,11 +2513,12 @@
       <c r="C149" s="1"/>
       <c r="D149" s="3"/>
       <c r="E149" s="3"/>
-      <c r="F149" s="4"/>
+      <c r="F149" s="3"/>
       <c r="G149" s="4"/>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
-      <c r="J149" s="3"/>
+      <c r="J149" s="4"/>
+      <c r="K149" s="3"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3"/>
@@ -2373,11 +2526,12 @@
       <c r="C150" s="1"/>
       <c r="D150" s="3"/>
       <c r="E150" s="3"/>
-      <c r="F150" s="4"/>
+      <c r="F150" s="3"/>
       <c r="G150" s="4"/>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
-      <c r="J150" s="3"/>
+      <c r="J150" s="4"/>
+      <c r="K150" s="3"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3"/>
@@ -2385,11 +2539,12 @@
       <c r="C151" s="1"/>
       <c r="D151" s="3"/>
       <c r="E151" s="3"/>
-      <c r="F151" s="4"/>
+      <c r="F151" s="3"/>
       <c r="G151" s="4"/>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
-      <c r="J151" s="3"/>
+      <c r="J151" s="4"/>
+      <c r="K151" s="3"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="3"/>
@@ -2397,11 +2552,12 @@
       <c r="C152" s="1"/>
       <c r="D152" s="3"/>
       <c r="E152" s="3"/>
-      <c r="F152" s="4"/>
+      <c r="F152" s="3"/>
       <c r="G152" s="4"/>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
-      <c r="J152" s="3"/>
+      <c r="J152" s="4"/>
+      <c r="K152" s="3"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3"/>
@@ -2409,11 +2565,12 @@
       <c r="C153" s="1"/>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
-      <c r="F153" s="4"/>
+      <c r="F153" s="3"/>
       <c r="G153" s="4"/>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
-      <c r="J153" s="3"/>
+      <c r="J153" s="4"/>
+      <c r="K153" s="3"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3"/>
@@ -2421,11 +2578,12 @@
       <c r="C154" s="1"/>
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
-      <c r="F154" s="4"/>
+      <c r="F154" s="3"/>
       <c r="G154" s="4"/>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
-      <c r="J154" s="3"/>
+      <c r="J154" s="4"/>
+      <c r="K154" s="3"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="3"/>
@@ -2433,11 +2591,12 @@
       <c r="C155" s="1"/>
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
-      <c r="F155" s="4"/>
+      <c r="F155" s="3"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
-      <c r="J155" s="3"/>
+      <c r="J155" s="4"/>
+      <c r="K155" s="3"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="3"/>
@@ -2445,11 +2604,12 @@
       <c r="C156" s="1"/>
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
-      <c r="F156" s="4"/>
+      <c r="F156" s="3"/>
       <c r="G156" s="4"/>
       <c r="H156" s="4"/>
       <c r="I156" s="4"/>
-      <c r="J156" s="3"/>
+      <c r="J156" s="4"/>
+      <c r="K156" s="3"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="3"/>
@@ -2457,11 +2617,12 @@
       <c r="C157" s="1"/>
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
-      <c r="F157" s="4"/>
+      <c r="F157" s="3"/>
       <c r="G157" s="4"/>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
-      <c r="J157" s="3"/>
+      <c r="J157" s="4"/>
+      <c r="K157" s="3"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="3"/>
@@ -2469,11 +2630,12 @@
       <c r="C158" s="1"/>
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
-      <c r="F158" s="4"/>
+      <c r="F158" s="3"/>
       <c r="G158" s="4"/>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
-      <c r="J158" s="3"/>
+      <c r="J158" s="4"/>
+      <c r="K158" s="3"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="3"/>
@@ -2481,11 +2643,12 @@
       <c r="C159" s="1"/>
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
-      <c r="F159" s="4"/>
+      <c r="F159" s="3"/>
       <c r="G159" s="4"/>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
-      <c r="J159" s="3"/>
+      <c r="J159" s="4"/>
+      <c r="K159" s="3"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="3"/>
@@ -2493,11 +2656,12 @@
       <c r="C160" s="1"/>
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
-      <c r="F160" s="4"/>
+      <c r="F160" s="3"/>
       <c r="G160" s="4"/>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
-      <c r="J160" s="3"/>
+      <c r="J160" s="4"/>
+      <c r="K160" s="3"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="3"/>
@@ -2505,11 +2669,12 @@
       <c r="C161" s="1"/>
       <c r="D161" s="3"/>
       <c r="E161" s="3"/>
-      <c r="F161" s="4"/>
+      <c r="F161" s="3"/>
       <c r="G161" s="4"/>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
-      <c r="J161" s="3"/>
+      <c r="J161" s="4"/>
+      <c r="K161" s="3"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="3"/>
@@ -2517,11 +2682,12 @@
       <c r="C162" s="1"/>
       <c r="D162" s="3"/>
       <c r="E162" s="3"/>
-      <c r="F162" s="4"/>
+      <c r="F162" s="3"/>
       <c r="G162" s="4"/>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
-      <c r="J162" s="3"/>
+      <c r="J162" s="4"/>
+      <c r="K162" s="3"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="3"/>
@@ -2529,11 +2695,12 @@
       <c r="C163" s="1"/>
       <c r="D163" s="3"/>
       <c r="E163" s="3"/>
-      <c r="F163" s="4"/>
+      <c r="F163" s="3"/>
       <c r="G163" s="4"/>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
-      <c r="J163" s="3"/>
+      <c r="J163" s="4"/>
+      <c r="K163" s="3"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="3"/>
@@ -2541,11 +2708,12 @@
       <c r="C164" s="1"/>
       <c r="D164" s="3"/>
       <c r="E164" s="3"/>
-      <c r="F164" s="4"/>
+      <c r="F164" s="3"/>
       <c r="G164" s="4"/>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
-      <c r="J164" s="3"/>
+      <c r="J164" s="4"/>
+      <c r="K164" s="3"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="3"/>
@@ -2553,11 +2721,12 @@
       <c r="C165" s="1"/>
       <c r="D165" s="3"/>
       <c r="E165" s="3"/>
-      <c r="F165" s="4"/>
+      <c r="F165" s="3"/>
       <c r="G165" s="4"/>
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
-      <c r="J165" s="3"/>
+      <c r="J165" s="4"/>
+      <c r="K165" s="3"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="3"/>
@@ -2565,11 +2734,12 @@
       <c r="C166" s="1"/>
       <c r="D166" s="3"/>
       <c r="E166" s="3"/>
-      <c r="F166" s="4"/>
+      <c r="F166" s="3"/>
       <c r="G166" s="4"/>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
-      <c r="J166" s="3"/>
+      <c r="J166" s="4"/>
+      <c r="K166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="3"/>
@@ -2577,11 +2747,12 @@
       <c r="C167" s="1"/>
       <c r="D167" s="3"/>
       <c r="E167" s="3"/>
-      <c r="F167" s="4"/>
+      <c r="F167" s="3"/>
       <c r="G167" s="4"/>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
-      <c r="J167" s="3"/>
+      <c r="J167" s="4"/>
+      <c r="K167" s="3"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="3"/>
@@ -2589,11 +2760,12 @@
       <c r="C168" s="1"/>
       <c r="D168" s="3"/>
       <c r="E168" s="3"/>
-      <c r="F168" s="4"/>
+      <c r="F168" s="3"/>
       <c r="G168" s="4"/>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
-      <c r="J168" s="3"/>
+      <c r="J168" s="4"/>
+      <c r="K168" s="3"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="3"/>
@@ -2601,11 +2773,12 @@
       <c r="C169" s="1"/>
       <c r="D169" s="3"/>
       <c r="E169" s="3"/>
-      <c r="F169" s="4"/>
+      <c r="F169" s="3"/>
       <c r="G169" s="4"/>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
-      <c r="J169" s="3"/>
+      <c r="J169" s="4"/>
+      <c r="K169" s="3"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="3"/>
@@ -2613,11 +2786,12 @@
       <c r="C170" s="1"/>
       <c r="D170" s="3"/>
       <c r="E170" s="3"/>
-      <c r="F170" s="4"/>
+      <c r="F170" s="3"/>
       <c r="G170" s="4"/>
       <c r="H170" s="4"/>
       <c r="I170" s="4"/>
-      <c r="J170" s="3"/>
+      <c r="J170" s="4"/>
+      <c r="K170" s="3"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="3"/>
@@ -2625,11 +2799,12 @@
       <c r="C171" s="1"/>
       <c r="D171" s="3"/>
       <c r="E171" s="3"/>
-      <c r="F171" s="4"/>
+      <c r="F171" s="3"/>
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
-      <c r="J171" s="3"/>
+      <c r="J171" s="4"/>
+      <c r="K171" s="3"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="3"/>
@@ -2637,11 +2812,12 @@
       <c r="C172" s="1"/>
       <c r="D172" s="3"/>
       <c r="E172" s="3"/>
-      <c r="F172" s="4"/>
+      <c r="F172" s="3"/>
       <c r="G172" s="4"/>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
-      <c r="J172" s="3"/>
+      <c r="J172" s="4"/>
+      <c r="K172" s="3"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="3"/>
@@ -2649,11 +2825,12 @@
       <c r="C173" s="1"/>
       <c r="D173" s="3"/>
       <c r="E173" s="3"/>
-      <c r="F173" s="4"/>
+      <c r="F173" s="3"/>
       <c r="G173" s="4"/>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
-      <c r="J173" s="3"/>
+      <c r="J173" s="4"/>
+      <c r="K173" s="3"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="3"/>
@@ -2661,11 +2838,12 @@
       <c r="C174" s="1"/>
       <c r="D174" s="3"/>
       <c r="E174" s="3"/>
-      <c r="F174" s="4"/>
+      <c r="F174" s="3"/>
       <c r="G174" s="4"/>
       <c r="H174" s="4"/>
       <c r="I174" s="4"/>
-      <c r="J174" s="3"/>
+      <c r="J174" s="4"/>
+      <c r="K174" s="3"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="3"/>
@@ -2673,11 +2851,12 @@
       <c r="C175" s="1"/>
       <c r="D175" s="3"/>
       <c r="E175" s="3"/>
-      <c r="F175" s="4"/>
+      <c r="F175" s="3"/>
       <c r="G175" s="4"/>
       <c r="H175" s="4"/>
       <c r="I175" s="4"/>
-      <c r="J175" s="3"/>
+      <c r="J175" s="4"/>
+      <c r="K175" s="3"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="3"/>
@@ -2685,11 +2864,12 @@
       <c r="C176" s="1"/>
       <c r="D176" s="3"/>
       <c r="E176" s="3"/>
-      <c r="F176" s="4"/>
+      <c r="F176" s="3"/>
       <c r="G176" s="4"/>
       <c r="H176" s="4"/>
       <c r="I176" s="4"/>
-      <c r="J176" s="3"/>
+      <c r="J176" s="4"/>
+      <c r="K176" s="3"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="3"/>
@@ -2697,11 +2877,12 @@
       <c r="C177" s="1"/>
       <c r="D177" s="3"/>
       <c r="E177" s="3"/>
-      <c r="F177" s="4"/>
+      <c r="F177" s="3"/>
       <c r="G177" s="4"/>
       <c r="H177" s="4"/>
       <c r="I177" s="4"/>
-      <c r="J177" s="3"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="3"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="3"/>
@@ -2709,11 +2890,12 @@
       <c r="C178" s="1"/>
       <c r="D178" s="3"/>
       <c r="E178" s="3"/>
-      <c r="F178" s="4"/>
+      <c r="F178" s="3"/>
       <c r="G178" s="4"/>
       <c r="H178" s="4"/>
       <c r="I178" s="4"/>
-      <c r="J178" s="3"/>
+      <c r="J178" s="4"/>
+      <c r="K178" s="3"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="3"/>
@@ -2721,11 +2903,12 @@
       <c r="C179" s="1"/>
       <c r="D179" s="3"/>
       <c r="E179" s="3"/>
-      <c r="F179" s="4"/>
+      <c r="F179" s="3"/>
       <c r="G179" s="4"/>
       <c r="H179" s="4"/>
       <c r="I179" s="4"/>
-      <c r="J179" s="3"/>
+      <c r="J179" s="4"/>
+      <c r="K179" s="3"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="3"/>
@@ -2733,11 +2916,12 @@
       <c r="C180" s="1"/>
       <c r="D180" s="3"/>
       <c r="E180" s="3"/>
-      <c r="F180" s="4"/>
+      <c r="F180" s="3"/>
       <c r="G180" s="4"/>
       <c r="H180" s="4"/>
       <c r="I180" s="4"/>
-      <c r="J180" s="3"/>
+      <c r="J180" s="4"/>
+      <c r="K180" s="3"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="3"/>
@@ -2745,11 +2929,12 @@
       <c r="C181" s="1"/>
       <c r="D181" s="3"/>
       <c r="E181" s="3"/>
-      <c r="F181" s="4"/>
+      <c r="F181" s="3"/>
       <c r="G181" s="4"/>
       <c r="H181" s="4"/>
       <c r="I181" s="4"/>
-      <c r="J181" s="3"/>
+      <c r="J181" s="4"/>
+      <c r="K181" s="3"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="3"/>
@@ -2757,11 +2942,12 @@
       <c r="C182" s="1"/>
       <c r="D182" s="3"/>
       <c r="E182" s="3"/>
-      <c r="F182" s="4"/>
+      <c r="F182" s="3"/>
       <c r="G182" s="4"/>
       <c r="H182" s="4"/>
       <c r="I182" s="4"/>
-      <c r="J182" s="3"/>
+      <c r="J182" s="4"/>
+      <c r="K182" s="3"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="3"/>
@@ -2769,11 +2955,12 @@
       <c r="C183" s="1"/>
       <c r="D183" s="3"/>
       <c r="E183" s="3"/>
-      <c r="F183" s="4"/>
+      <c r="F183" s="3"/>
       <c r="G183" s="4"/>
       <c r="H183" s="4"/>
       <c r="I183" s="4"/>
-      <c r="J183" s="3"/>
+      <c r="J183" s="4"/>
+      <c r="K183" s="3"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="3"/>
@@ -2781,11 +2968,12 @@
       <c r="C184" s="1"/>
       <c r="D184" s="3"/>
       <c r="E184" s="3"/>
-      <c r="F184" s="4"/>
+      <c r="F184" s="3"/>
       <c r="G184" s="4"/>
       <c r="H184" s="4"/>
       <c r="I184" s="4"/>
-      <c r="J184" s="3"/>
+      <c r="J184" s="4"/>
+      <c r="K184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="3"/>
@@ -2793,11 +2981,12 @@
       <c r="C185" s="1"/>
       <c r="D185" s="3"/>
       <c r="E185" s="3"/>
-      <c r="F185" s="4"/>
+      <c r="F185" s="3"/>
       <c r="G185" s="4"/>
       <c r="H185" s="4"/>
       <c r="I185" s="4"/>
-      <c r="J185" s="3"/>
+      <c r="J185" s="4"/>
+      <c r="K185" s="3"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="3"/>
@@ -2805,11 +2994,12 @@
       <c r="C186" s="1"/>
       <c r="D186" s="3"/>
       <c r="E186" s="3"/>
-      <c r="F186" s="4"/>
+      <c r="F186" s="3"/>
       <c r="G186" s="4"/>
       <c r="H186" s="4"/>
       <c r="I186" s="4"/>
-      <c r="J186" s="3"/>
+      <c r="J186" s="4"/>
+      <c r="K186" s="3"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="3"/>
@@ -2817,11 +3007,12 @@
       <c r="C187" s="1"/>
       <c r="D187" s="3"/>
       <c r="E187" s="3"/>
-      <c r="F187" s="4"/>
+      <c r="F187" s="3"/>
       <c r="G187" s="4"/>
       <c r="H187" s="4"/>
       <c r="I187" s="4"/>
-      <c r="J187" s="3"/>
+      <c r="J187" s="4"/>
+      <c r="K187" s="3"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="3"/>
@@ -2829,11 +3020,12 @@
       <c r="C188" s="1"/>
       <c r="D188" s="3"/>
       <c r="E188" s="3"/>
-      <c r="F188" s="4"/>
+      <c r="F188" s="3"/>
       <c r="G188" s="4"/>
       <c r="H188" s="4"/>
       <c r="I188" s="4"/>
-      <c r="J188" s="3"/>
+      <c r="J188" s="4"/>
+      <c r="K188" s="3"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="3"/>
@@ -2841,11 +3033,12 @@
       <c r="C189" s="1"/>
       <c r="D189" s="3"/>
       <c r="E189" s="3"/>
-      <c r="F189" s="4"/>
+      <c r="F189" s="3"/>
       <c r="G189" s="4"/>
       <c r="H189" s="4"/>
       <c r="I189" s="4"/>
-      <c r="J189" s="3"/>
+      <c r="J189" s="4"/>
+      <c r="K189" s="3"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="3"/>
@@ -2853,11 +3046,12 @@
       <c r="C190" s="1"/>
       <c r="D190" s="3"/>
       <c r="E190" s="3"/>
-      <c r="F190" s="4"/>
+      <c r="F190" s="3"/>
       <c r="G190" s="4"/>
       <c r="H190" s="4"/>
       <c r="I190" s="4"/>
-      <c r="J190" s="3"/>
+      <c r="J190" s="4"/>
+      <c r="K190" s="3"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="3"/>
@@ -2865,11 +3059,12 @@
       <c r="C191" s="1"/>
       <c r="D191" s="3"/>
       <c r="E191" s="3"/>
-      <c r="F191" s="4"/>
+      <c r="F191" s="3"/>
       <c r="G191" s="4"/>
       <c r="H191" s="4"/>
       <c r="I191" s="4"/>
-      <c r="J191" s="3"/>
+      <c r="J191" s="4"/>
+      <c r="K191" s="3"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="3"/>
@@ -2877,11 +3072,12 @@
       <c r="C192" s="1"/>
       <c r="D192" s="3"/>
       <c r="E192" s="3"/>
-      <c r="F192" s="4"/>
+      <c r="F192" s="3"/>
       <c r="G192" s="4"/>
       <c r="H192" s="4"/>
       <c r="I192" s="4"/>
-      <c r="J192" s="3"/>
+      <c r="J192" s="4"/>
+      <c r="K192" s="3"/>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="3"/>
@@ -2889,11 +3085,12 @@
       <c r="C193" s="1"/>
       <c r="D193" s="3"/>
       <c r="E193" s="3"/>
-      <c r="F193" s="4"/>
+      <c r="F193" s="3"/>
       <c r="G193" s="4"/>
       <c r="H193" s="4"/>
       <c r="I193" s="4"/>
-      <c r="J193" s="3"/>
+      <c r="J193" s="4"/>
+      <c r="K193" s="3"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="3"/>
@@ -2901,11 +3098,12 @@
       <c r="C194" s="1"/>
       <c r="D194" s="3"/>
       <c r="E194" s="3"/>
-      <c r="F194" s="4"/>
+      <c r="F194" s="3"/>
       <c r="G194" s="4"/>
       <c r="H194" s="4"/>
       <c r="I194" s="4"/>
-      <c r="J194" s="3"/>
+      <c r="J194" s="4"/>
+      <c r="K194" s="3"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="3"/>
@@ -2913,11 +3111,12 @@
       <c r="C195" s="1"/>
       <c r="D195" s="3"/>
       <c r="E195" s="3"/>
-      <c r="F195" s="4"/>
+      <c r="F195" s="3"/>
       <c r="G195" s="4"/>
       <c r="H195" s="4"/>
       <c r="I195" s="4"/>
-      <c r="J195" s="3"/>
+      <c r="J195" s="4"/>
+      <c r="K195" s="3"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="3"/>
@@ -2925,11 +3124,12 @@
       <c r="C196" s="1"/>
       <c r="D196" s="3"/>
       <c r="E196" s="3"/>
-      <c r="F196" s="4"/>
+      <c r="F196" s="3"/>
       <c r="G196" s="4"/>
       <c r="H196" s="4"/>
       <c r="I196" s="4"/>
-      <c r="J196" s="3"/>
+      <c r="J196" s="4"/>
+      <c r="K196" s="3"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="3"/>
@@ -2937,11 +3137,12 @@
       <c r="C197" s="1"/>
       <c r="D197" s="3"/>
       <c r="E197" s="3"/>
-      <c r="F197" s="4"/>
+      <c r="F197" s="3"/>
       <c r="G197" s="4"/>
       <c r="H197" s="4"/>
       <c r="I197" s="4"/>
-      <c r="J197" s="3"/>
+      <c r="J197" s="4"/>
+      <c r="K197" s="3"/>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="3"/>
@@ -2949,11 +3150,12 @@
       <c r="C198" s="1"/>
       <c r="D198" s="3"/>
       <c r="E198" s="3"/>
-      <c r="F198" s="4"/>
+      <c r="F198" s="3"/>
       <c r="G198" s="4"/>
       <c r="H198" s="4"/>
       <c r="I198" s="4"/>
-      <c r="J198" s="3"/>
+      <c r="J198" s="4"/>
+      <c r="K198" s="3"/>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="3"/>
@@ -2961,11 +3163,12 @@
       <c r="C199" s="1"/>
       <c r="D199" s="3"/>
       <c r="E199" s="3"/>
-      <c r="F199" s="4"/>
+      <c r="F199" s="3"/>
       <c r="G199" s="4"/>
       <c r="H199" s="4"/>
       <c r="I199" s="4"/>
-      <c r="J199" s="3"/>
+      <c r="J199" s="4"/>
+      <c r="K199" s="3"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="3"/>
@@ -2973,11 +3176,12 @@
       <c r="C200" s="1"/>
       <c r="D200" s="3"/>
       <c r="E200" s="3"/>
-      <c r="F200" s="4"/>
+      <c r="F200" s="3"/>
       <c r="G200" s="4"/>
       <c r="H200" s="4"/>
       <c r="I200" s="4"/>
-      <c r="J200" s="3"/>
+      <c r="J200" s="4"/>
+      <c r="K200" s="3"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="3"/>
@@ -2985,11 +3189,12 @@
       <c r="C201" s="1"/>
       <c r="D201" s="3"/>
       <c r="E201" s="3"/>
-      <c r="F201" s="4"/>
+      <c r="F201" s="3"/>
       <c r="G201" s="4"/>
       <c r="H201" s="4"/>
       <c r="I201" s="4"/>
-      <c r="J201" s="3"/>
+      <c r="J201" s="4"/>
+      <c r="K201" s="3"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="3"/>
@@ -2997,11 +3202,12 @@
       <c r="C202" s="1"/>
       <c r="D202" s="3"/>
       <c r="E202" s="3"/>
-      <c r="F202" s="4"/>
+      <c r="F202" s="3"/>
       <c r="G202" s="4"/>
       <c r="H202" s="4"/>
       <c r="I202" s="4"/>
-      <c r="J202" s="3"/>
+      <c r="J202" s="4"/>
+      <c r="K202" s="3"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="3"/>
@@ -3009,11 +3215,12 @@
       <c r="C203" s="1"/>
       <c r="D203" s="3"/>
       <c r="E203" s="3"/>
-      <c r="F203" s="4"/>
+      <c r="F203" s="3"/>
       <c r="G203" s="4"/>
       <c r="H203" s="4"/>
       <c r="I203" s="4"/>
-      <c r="J203" s="3"/>
+      <c r="J203" s="4"/>
+      <c r="K203" s="3"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="3"/>
@@ -3021,11 +3228,12 @@
       <c r="C204" s="1"/>
       <c r="D204" s="3"/>
       <c r="E204" s="3"/>
-      <c r="F204" s="4"/>
+      <c r="F204" s="3"/>
       <c r="G204" s="4"/>
       <c r="H204" s="4"/>
       <c r="I204" s="4"/>
-      <c r="J204" s="3"/>
+      <c r="J204" s="4"/>
+      <c r="K204" s="3"/>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="3"/>
@@ -3033,11 +3241,12 @@
       <c r="C205" s="1"/>
       <c r="D205" s="3"/>
       <c r="E205" s="3"/>
-      <c r="F205" s="4"/>
+      <c r="F205" s="3"/>
       <c r="G205" s="4"/>
       <c r="H205" s="4"/>
       <c r="I205" s="4"/>
-      <c r="J205" s="3"/>
+      <c r="J205" s="4"/>
+      <c r="K205" s="3"/>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="3"/>
@@ -3045,11 +3254,12 @@
       <c r="C206" s="1"/>
       <c r="D206" s="3"/>
       <c r="E206" s="3"/>
-      <c r="F206" s="4"/>
+      <c r="F206" s="3"/>
       <c r="G206" s="4"/>
       <c r="H206" s="4"/>
       <c r="I206" s="4"/>
-      <c r="J206" s="3"/>
+      <c r="J206" s="4"/>
+      <c r="K206" s="3"/>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="3"/>
@@ -3057,11 +3267,12 @@
       <c r="C207" s="1"/>
       <c r="D207" s="3"/>
       <c r="E207" s="3"/>
-      <c r="F207" s="4"/>
+      <c r="F207" s="3"/>
       <c r="G207" s="4"/>
       <c r="H207" s="4"/>
       <c r="I207" s="4"/>
-      <c r="J207" s="3"/>
+      <c r="J207" s="4"/>
+      <c r="K207" s="3"/>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="3"/>
@@ -3069,11 +3280,12 @@
       <c r="C208" s="1"/>
       <c r="D208" s="3"/>
       <c r="E208" s="3"/>
-      <c r="F208" s="4"/>
+      <c r="F208" s="3"/>
       <c r="G208" s="4"/>
       <c r="H208" s="4"/>
       <c r="I208" s="4"/>
-      <c r="J208" s="3"/>
+      <c r="J208" s="4"/>
+      <c r="K208" s="3"/>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="3"/>
@@ -3081,11 +3293,12 @@
       <c r="C209" s="1"/>
       <c r="D209" s="3"/>
       <c r="E209" s="3"/>
-      <c r="F209" s="4"/>
+      <c r="F209" s="3"/>
       <c r="G209" s="4"/>
       <c r="H209" s="4"/>
       <c r="I209" s="4"/>
-      <c r="J209" s="3"/>
+      <c r="J209" s="4"/>
+      <c r="K209" s="3"/>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="3"/>
@@ -3093,11 +3306,12 @@
       <c r="C210" s="1"/>
       <c r="D210" s="3"/>
       <c r="E210" s="3"/>
-      <c r="F210" s="4"/>
+      <c r="F210" s="3"/>
       <c r="G210" s="4"/>
       <c r="H210" s="4"/>
       <c r="I210" s="4"/>
-      <c r="J210" s="3"/>
+      <c r="J210" s="4"/>
+      <c r="K210" s="3"/>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="3"/>
@@ -3105,11 +3319,12 @@
       <c r="C211" s="1"/>
       <c r="D211" s="3"/>
       <c r="E211" s="3"/>
-      <c r="F211" s="4"/>
+      <c r="F211" s="3"/>
       <c r="G211" s="4"/>
       <c r="H211" s="4"/>
       <c r="I211" s="4"/>
-      <c r="J211" s="3"/>
+      <c r="J211" s="4"/>
+      <c r="K211" s="3"/>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="3"/>
@@ -3117,11 +3332,12 @@
       <c r="C212" s="1"/>
       <c r="D212" s="3"/>
       <c r="E212" s="3"/>
-      <c r="F212" s="4"/>
+      <c r="F212" s="3"/>
       <c r="G212" s="4"/>
       <c r="H212" s="4"/>
       <c r="I212" s="4"/>
-      <c r="J212" s="3"/>
+      <c r="J212" s="4"/>
+      <c r="K212" s="3"/>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="3"/>
@@ -3129,11 +3345,12 @@
       <c r="C213" s="1"/>
       <c r="D213" s="3"/>
       <c r="E213" s="3"/>
-      <c r="F213" s="4"/>
+      <c r="F213" s="3"/>
       <c r="G213" s="4"/>
       <c r="H213" s="4"/>
       <c r="I213" s="4"/>
-      <c r="J213" s="3"/>
+      <c r="J213" s="4"/>
+      <c r="K213" s="3"/>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="3"/>
@@ -3141,11 +3358,12 @@
       <c r="C214" s="1"/>
       <c r="D214" s="3"/>
       <c r="E214" s="3"/>
-      <c r="F214" s="4"/>
+      <c r="F214" s="3"/>
       <c r="G214" s="4"/>
       <c r="H214" s="4"/>
       <c r="I214" s="4"/>
-      <c r="J214" s="3"/>
+      <c r="J214" s="4"/>
+      <c r="K214" s="3"/>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="3"/>
@@ -3153,11 +3371,12 @@
       <c r="C215" s="1"/>
       <c r="D215" s="3"/>
       <c r="E215" s="3"/>
-      <c r="F215" s="4"/>
+      <c r="F215" s="3"/>
       <c r="G215" s="4"/>
       <c r="H215" s="4"/>
       <c r="I215" s="4"/>
-      <c r="J215" s="3"/>
+      <c r="J215" s="4"/>
+      <c r="K215" s="3"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="3"/>
@@ -3165,11 +3384,12 @@
       <c r="C216" s="1"/>
       <c r="D216" s="3"/>
       <c r="E216" s="3"/>
-      <c r="F216" s="4"/>
+      <c r="F216" s="3"/>
       <c r="G216" s="4"/>
       <c r="H216" s="4"/>
       <c r="I216" s="4"/>
-      <c r="J216" s="3"/>
+      <c r="J216" s="4"/>
+      <c r="K216" s="3"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="3"/>
@@ -3177,11 +3397,12 @@
       <c r="C217" s="1"/>
       <c r="D217" s="3"/>
       <c r="E217" s="3"/>
-      <c r="F217" s="4"/>
+      <c r="F217" s="3"/>
       <c r="G217" s="4"/>
       <c r="H217" s="4"/>
       <c r="I217" s="4"/>
-      <c r="J217" s="3"/>
+      <c r="J217" s="4"/>
+      <c r="K217" s="3"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="3"/>
@@ -3189,11 +3410,12 @@
       <c r="C218" s="1"/>
       <c r="D218" s="3"/>
       <c r="E218" s="3"/>
-      <c r="F218" s="4"/>
+      <c r="F218" s="3"/>
       <c r="G218" s="4"/>
       <c r="H218" s="4"/>
       <c r="I218" s="4"/>
-      <c r="J218" s="3"/>
+      <c r="J218" s="4"/>
+      <c r="K218" s="3"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="3"/>
@@ -3201,11 +3423,12 @@
       <c r="C219" s="1"/>
       <c r="D219" s="3"/>
       <c r="E219" s="3"/>
-      <c r="F219" s="4"/>
+      <c r="F219" s="3"/>
       <c r="G219" s="4"/>
       <c r="H219" s="4"/>
       <c r="I219" s="4"/>
-      <c r="J219" s="3"/>
+      <c r="J219" s="4"/>
+      <c r="K219" s="3"/>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="3"/>
@@ -3213,11 +3436,12 @@
       <c r="C220" s="1"/>
       <c r="D220" s="3"/>
       <c r="E220" s="3"/>
-      <c r="F220" s="4"/>
+      <c r="F220" s="3"/>
       <c r="G220" s="4"/>
       <c r="H220" s="4"/>
       <c r="I220" s="4"/>
-      <c r="J220" s="3"/>
+      <c r="J220" s="4"/>
+      <c r="K220" s="3"/>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="3"/>
@@ -3225,11 +3449,12 @@
       <c r="C221" s="1"/>
       <c r="D221" s="3"/>
       <c r="E221" s="3"/>
-      <c r="F221" s="4"/>
+      <c r="F221" s="3"/>
       <c r="G221" s="4"/>
       <c r="H221" s="4"/>
       <c r="I221" s="4"/>
-      <c r="J221" s="3"/>
+      <c r="J221" s="4"/>
+      <c r="K221" s="3"/>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="3"/>
@@ -3237,11 +3462,12 @@
       <c r="C222" s="1"/>
       <c r="D222" s="3"/>
       <c r="E222" s="3"/>
-      <c r="F222" s="4"/>
+      <c r="F222" s="3"/>
       <c r="G222" s="4"/>
       <c r="H222" s="4"/>
       <c r="I222" s="4"/>
-      <c r="J222" s="3"/>
+      <c r="J222" s="4"/>
+      <c r="K222" s="3"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="3"/>
@@ -3249,11 +3475,12 @@
       <c r="C223" s="1"/>
       <c r="D223" s="3"/>
       <c r="E223" s="3"/>
-      <c r="F223" s="4"/>
+      <c r="F223" s="3"/>
       <c r="G223" s="4"/>
       <c r="H223" s="4"/>
       <c r="I223" s="4"/>
-      <c r="J223" s="3"/>
+      <c r="J223" s="4"/>
+      <c r="K223" s="3"/>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="3"/>
@@ -3261,11 +3488,12 @@
       <c r="C224" s="1"/>
       <c r="D224" s="3"/>
       <c r="E224" s="3"/>
-      <c r="F224" s="4"/>
+      <c r="F224" s="3"/>
       <c r="G224" s="4"/>
       <c r="H224" s="4"/>
       <c r="I224" s="4"/>
-      <c r="J224" s="3"/>
+      <c r="J224" s="4"/>
+      <c r="K224" s="3"/>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="3"/>
@@ -3273,11 +3501,12 @@
       <c r="C225" s="1"/>
       <c r="D225" s="3"/>
       <c r="E225" s="3"/>
-      <c r="F225" s="4"/>
+      <c r="F225" s="3"/>
       <c r="G225" s="4"/>
       <c r="H225" s="4"/>
       <c r="I225" s="4"/>
-      <c r="J225" s="3"/>
+      <c r="J225" s="4"/>
+      <c r="K225" s="3"/>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="3"/>
@@ -3285,11 +3514,12 @@
       <c r="C226" s="1"/>
       <c r="D226" s="3"/>
       <c r="E226" s="3"/>
-      <c r="F226" s="4"/>
+      <c r="F226" s="3"/>
       <c r="G226" s="4"/>
       <c r="H226" s="4"/>
       <c r="I226" s="4"/>
-      <c r="J226" s="3"/>
+      <c r="J226" s="4"/>
+      <c r="K226" s="3"/>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="3"/>
@@ -3297,11 +3527,12 @@
       <c r="C227" s="1"/>
       <c r="D227" s="3"/>
       <c r="E227" s="3"/>
-      <c r="F227" s="4"/>
+      <c r="F227" s="3"/>
       <c r="G227" s="4"/>
       <c r="H227" s="4"/>
       <c r="I227" s="4"/>
-      <c r="J227" s="3"/>
+      <c r="J227" s="4"/>
+      <c r="K227" s="3"/>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="3"/>
@@ -3309,11 +3540,12 @@
       <c r="C228" s="1"/>
       <c r="D228" s="3"/>
       <c r="E228" s="3"/>
-      <c r="F228" s="4"/>
+      <c r="F228" s="3"/>
       <c r="G228" s="4"/>
       <c r="H228" s="4"/>
       <c r="I228" s="4"/>
-      <c r="J228" s="3"/>
+      <c r="J228" s="4"/>
+      <c r="K228" s="3"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="3"/>
@@ -3321,11 +3553,12 @@
       <c r="C229" s="1"/>
       <c r="D229" s="3"/>
       <c r="E229" s="3"/>
-      <c r="F229" s="4"/>
+      <c r="F229" s="3"/>
       <c r="G229" s="4"/>
       <c r="H229" s="4"/>
       <c r="I229" s="4"/>
-      <c r="J229" s="3"/>
+      <c r="J229" s="4"/>
+      <c r="K229" s="3"/>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="3"/>
@@ -3333,11 +3566,12 @@
       <c r="C230" s="1"/>
       <c r="D230" s="3"/>
       <c r="E230" s="3"/>
-      <c r="F230" s="4"/>
+      <c r="F230" s="3"/>
       <c r="G230" s="4"/>
       <c r="H230" s="4"/>
       <c r="I230" s="4"/>
-      <c r="J230" s="3"/>
+      <c r="J230" s="4"/>
+      <c r="K230" s="3"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="3"/>
@@ -3345,11 +3579,12 @@
       <c r="C231" s="1"/>
       <c r="D231" s="3"/>
       <c r="E231" s="3"/>
-      <c r="F231" s="4"/>
+      <c r="F231" s="3"/>
       <c r="G231" s="4"/>
       <c r="H231" s="4"/>
       <c r="I231" s="4"/>
-      <c r="J231" s="3"/>
+      <c r="J231" s="4"/>
+      <c r="K231" s="3"/>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="3"/>
@@ -3357,11 +3592,12 @@
       <c r="C232" s="1"/>
       <c r="D232" s="3"/>
       <c r="E232" s="3"/>
-      <c r="F232" s="4"/>
+      <c r="F232" s="3"/>
       <c r="G232" s="4"/>
       <c r="H232" s="4"/>
       <c r="I232" s="4"/>
-      <c r="J232" s="3"/>
+      <c r="J232" s="4"/>
+      <c r="K232" s="3"/>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="3"/>
@@ -3369,11 +3605,12 @@
       <c r="C233" s="1"/>
       <c r="D233" s="3"/>
       <c r="E233" s="3"/>
-      <c r="F233" s="4"/>
+      <c r="F233" s="3"/>
       <c r="G233" s="4"/>
       <c r="H233" s="4"/>
       <c r="I233" s="4"/>
-      <c r="J233" s="3"/>
+      <c r="J233" s="4"/>
+      <c r="K233" s="3"/>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="3"/>
@@ -3381,11 +3618,12 @@
       <c r="C234" s="1"/>
       <c r="D234" s="3"/>
       <c r="E234" s="3"/>
-      <c r="F234" s="4"/>
+      <c r="F234" s="3"/>
       <c r="G234" s="4"/>
       <c r="H234" s="4"/>
       <c r="I234" s="4"/>
-      <c r="J234" s="3"/>
+      <c r="J234" s="4"/>
+      <c r="K234" s="3"/>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="3"/>
@@ -3393,11 +3631,12 @@
       <c r="C235" s="1"/>
       <c r="D235" s="3"/>
       <c r="E235" s="3"/>
-      <c r="F235" s="4"/>
+      <c r="F235" s="3"/>
       <c r="G235" s="4"/>
       <c r="H235" s="4"/>
       <c r="I235" s="4"/>
-      <c r="J235" s="3"/>
+      <c r="J235" s="4"/>
+      <c r="K235" s="3"/>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="3"/>
@@ -3405,11 +3644,12 @@
       <c r="C236" s="1"/>
       <c r="D236" s="3"/>
       <c r="E236" s="3"/>
-      <c r="F236" s="4"/>
+      <c r="F236" s="3"/>
       <c r="G236" s="4"/>
       <c r="H236" s="4"/>
       <c r="I236" s="4"/>
-      <c r="J236" s="3"/>
+      <c r="J236" s="4"/>
+      <c r="K236" s="3"/>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="3"/>
@@ -3417,11 +3657,12 @@
       <c r="C237" s="1"/>
       <c r="D237" s="3"/>
       <c r="E237" s="3"/>
-      <c r="F237" s="4"/>
+      <c r="F237" s="3"/>
       <c r="G237" s="4"/>
       <c r="H237" s="4"/>
       <c r="I237" s="4"/>
-      <c r="J237" s="3"/>
+      <c r="J237" s="4"/>
+      <c r="K237" s="3"/>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="3"/>
@@ -3429,11 +3670,12 @@
       <c r="C238" s="1"/>
       <c r="D238" s="3"/>
       <c r="E238" s="3"/>
-      <c r="F238" s="4"/>
+      <c r="F238" s="3"/>
       <c r="G238" s="4"/>
       <c r="H238" s="4"/>
       <c r="I238" s="4"/>
-      <c r="J238" s="3"/>
+      <c r="J238" s="4"/>
+      <c r="K238" s="3"/>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="3"/>
@@ -3441,11 +3683,12 @@
       <c r="C239" s="1"/>
       <c r="D239" s="3"/>
       <c r="E239" s="3"/>
-      <c r="F239" s="4"/>
+      <c r="F239" s="3"/>
       <c r="G239" s="4"/>
       <c r="H239" s="4"/>
       <c r="I239" s="4"/>
-      <c r="J239" s="3"/>
+      <c r="J239" s="4"/>
+      <c r="K239" s="3"/>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="3"/>
@@ -3453,11 +3696,12 @@
       <c r="C240" s="1"/>
       <c r="D240" s="3"/>
       <c r="E240" s="3"/>
-      <c r="F240" s="4"/>
+      <c r="F240" s="3"/>
       <c r="G240" s="4"/>
       <c r="H240" s="4"/>
       <c r="I240" s="4"/>
-      <c r="J240" s="3"/>
+      <c r="J240" s="4"/>
+      <c r="K240" s="3"/>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="3"/>
@@ -3465,11 +3709,12 @@
       <c r="C241" s="1"/>
       <c r="D241" s="3"/>
       <c r="E241" s="3"/>
-      <c r="F241" s="4"/>
+      <c r="F241" s="3"/>
       <c r="G241" s="4"/>
       <c r="H241" s="4"/>
       <c r="I241" s="4"/>
-      <c r="J241" s="3"/>
+      <c r="J241" s="4"/>
+      <c r="K241" s="3"/>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="3"/>
@@ -3477,11 +3722,12 @@
       <c r="C242" s="1"/>
       <c r="D242" s="3"/>
       <c r="E242" s="3"/>
-      <c r="F242" s="4"/>
+      <c r="F242" s="3"/>
       <c r="G242" s="4"/>
       <c r="H242" s="4"/>
       <c r="I242" s="4"/>
-      <c r="J242" s="3"/>
+      <c r="J242" s="4"/>
+      <c r="K242" s="3"/>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="3"/>
@@ -3489,11 +3735,12 @@
       <c r="C243" s="1"/>
       <c r="D243" s="3"/>
       <c r="E243" s="3"/>
-      <c r="F243" s="4"/>
+      <c r="F243" s="3"/>
       <c r="G243" s="4"/>
       <c r="H243" s="4"/>
       <c r="I243" s="4"/>
-      <c r="J243" s="3"/>
+      <c r="J243" s="4"/>
+      <c r="K243" s="3"/>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B244" s="3"/>
@@ -3664,9 +3911,9 @@
       <c r="B299" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:J243"/>
+  <autoFilter ref="B1:K243"/>
   <dataValidations count="8">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J351:J1001" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K351:K1001" type="list">
       <formula1>"Derslik,Bilgisayar Laboratuvarı,Uzaktan Eğitim Sınıfı,Karma"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3678,7 +3925,7 @@
       <formula1>"Bilgisayar Programcılığı,Web Tasarımı ve Kodlama,Elektrik Üretim İletim ve Dağıtım,Alternatif Enerji Kaynakları Teknolojisi,Geleneksel El Sanatları,Kuyumculuk ve Takı Tasarımı,Bankacılık ve Sigortacılık Programı,Maliye,Muhasebe Ve Vergi Uygulamaları,Turiz"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I350" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J350" type="list">
       <formula1>Sheet2!$C$2:$C$45</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3694,7 +3941,7 @@
       <formula1>Sheet2!$D$2:$D$9</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J350" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2:K350" type="list">
       <formula1>Sheet2!$E$2:$E$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3726,551 +3973,551 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="37.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="45.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="31.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>13</v>
+      <c r="E1" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>14</v>
+      <c r="A2" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="D2" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
-        <v>19</v>
+      <c r="A3" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>24</v>
+      <c r="A4" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="E4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>29</v>
+      <c r="A5" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="E5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>34</v>
+      <c r="A6" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>38</v>
+      <c r="A7" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="C7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>41</v>
+      <c r="A8" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="C8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>44</v>
+      <c r="A9" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="7" t="s">
         <v>46</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>47</v>
+      <c r="A10" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="C11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="C12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="C13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
+      <c r="C14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8"/>
+      <c r="C15" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="C16" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="C17" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="C18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="C19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="C20" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="C21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="C22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="8"/>
+      <c r="C23" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="7"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="C24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
+      <c r="C25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
       <c r="I25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="8"/>
+      <c r="C26" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="7"/>
       <c r="I26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="8"/>
+      <c r="C27" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="7"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
+      <c r="C28" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="7"/>
+      <c r="C29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="6"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
       <c r="I29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
+      <c r="C30" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="C31" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
       <c r="I31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="C32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
       <c r="I32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="8"/>
+      <c r="C33" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="7"/>
       <c r="I33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D34" s="7"/>
+      <c r="C34" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="6"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
       <c r="I34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="8"/>
+      <c r="C35" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="7"/>
       <c r="I35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
+      <c r="C36" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
       <c r="I36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
+      <c r="C37" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
       <c r="I37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
+      <c r="C38" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
       <c r="I38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="8"/>
+      <c r="C39" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="7"/>
       <c r="I39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="C40" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
       <c r="I40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
       <c r="I41" s="3"/>
     </row>
   </sheetData>

</xml_diff>